<commit_message>
Added interfaces between BluetoothConnection, Game, and GameView.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Planning</t>
   </si>
   <si>
-    <t>PLanning</t>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -69,7 +69,7 @@
     <numFmt numFmtId="165" formatCode="0&quot; mins&quot;"/>
     <numFmt numFmtId="166" formatCode="0.0#&quot; hours&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +79,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -103,10 +110,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -118,9 +126,12 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -193,13 +204,13 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3166666666666713</c:v>
+                  <c:v>9.033333333333335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4666666666666694</c:v>
+                  <c:v>2.0833333333333361</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6833333333333291</c:v>
+                  <c:v>4.0499999999999972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -233,16 +244,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -551,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,13 +574,14 @@
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -594,8 +606,11 @@
       <c r="I1" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>41879</v>
       </c>
@@ -622,8 +637,12 @@
         <f>SUMIF($F$2:$F$25,H2,$E$2:$E$25)</f>
         <v>1.6166666666666663</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="12">
+        <f>I2/SUM($I$2:$I$5)</f>
+        <v>9.6325719960278014E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>41880</v>
       </c>
@@ -647,11 +666,15 @@
         <v>7</v>
       </c>
       <c r="I3" s="10">
-        <f t="shared" ref="I3:I5" si="0">SUMIF($F$2:$F$25,H3,$E$2:$E$25)</f>
-        <v>2.3166666666666713</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <f>SUMIF($F$2:$F$25,H3,$E$2:$E$25)</f>
+        <v>9.033333333333335</v>
+      </c>
+      <c r="J3" s="12">
+        <f t="shared" ref="J3:J5" si="0">I3/SUM($I$2:$I$5)</f>
+        <v>0.53823237338629593</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>41880</v>
       </c>
@@ -675,11 +698,15 @@
         <v>8</v>
       </c>
       <c r="I4" s="10">
+        <f>SUMIF($F$2:$F$25,H4,$E$2:$E$25)</f>
+        <v>2.0833333333333361</v>
+      </c>
+      <c r="J4" s="12">
         <f t="shared" si="0"/>
-        <v>1.4666666666666694</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.12413108242303889</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>41880</v>
       </c>
@@ -703,11 +730,15 @@
         <v>12</v>
       </c>
       <c r="I5" s="10">
+        <f>SUMIF($F$2:$F$25,H5,$E$2:$E$25)</f>
+        <v>4.0499999999999972</v>
+      </c>
+      <c r="J5" s="12">
         <f t="shared" si="0"/>
-        <v>3.6833333333333291</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.24131082423038711</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>41880</v>
       </c>
@@ -728,7 +759,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>41880</v>
       </c>
@@ -749,7 +780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>41880</v>
       </c>
@@ -770,7 +801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>41881</v>
       </c>
@@ -791,7 +822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>41881</v>
       </c>
@@ -812,7 +843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>41882</v>
       </c>
@@ -830,100 +861,220 @@
         <v>1.45</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="4" t="str">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>41882</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.55069444444444449</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.61944444444444446</v>
+      </c>
+      <c r="D12" s="3">
+        <v>15</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="1"/>
+        <v>1.3999999999999995</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>41882</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.85277777777777775</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="1"/>
+        <v>1.1333333333333346</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>41882</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.94166666666666676</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.96527777777777779</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="1"/>
+        <v>0.56666666666666465</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>41883</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.58611111111111114</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.60486111111111118</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="1"/>
+        <v>0.36666666666666775</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>41883</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.60486111111111118</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.63472222222222219</v>
+      </c>
+      <c r="D16" s="3">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="1"/>
+        <v>0.63333333333333075</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>41883</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.72083333333333333</v>
+      </c>
+      <c r="D17" s="3">
+        <v>15</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999998</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>41883</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.92222222222222217</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="D18" s="3">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6833333333333347</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>41884</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2.7083333333333334E-2</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="1"/>
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="4" t="str">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="4" t="str">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="4" t="str">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="4" t="str">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="4" t="str">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="4">
         <f>SUM(E2:E25)</f>
-        <v>9.0833333333333357</v>
+        <v>16.783333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit before combining BluetoothConnection and BluetoothConnectionFragment.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -204,7 +204,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.033333333333335</c:v>
+                  <c:v>9.8500000000000014</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0833333333333361</c:v>
@@ -565,7 +565,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +639,7 @@
       </c>
       <c r="J2" s="12">
         <f>I2/SUM($I$2:$I$5)</f>
-        <v>9.6325719960278014E-2</v>
+        <v>9.185606060606058E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -667,11 +667,11 @@
       </c>
       <c r="I3" s="10">
         <f>SUMIF($F$2:$F$25,H3,$E$2:$E$25)</f>
-        <v>9.033333333333335</v>
+        <v>9.8500000000000014</v>
       </c>
       <c r="J3" s="12">
         <f t="shared" ref="J3:J5" si="0">I3/SUM($I$2:$I$5)</f>
-        <v>0.53823237338629593</v>
+        <v>0.55965909090909094</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
       </c>
       <c r="J4" s="12">
         <f t="shared" si="0"/>
-        <v>0.12413108242303889</v>
+        <v>0.11837121212121227</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -735,7 +735,7 @@
       </c>
       <c r="J5" s="12">
         <f t="shared" si="0"/>
-        <v>0.24131082423038711</v>
+        <v>0.23011363636363619</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1033,9 +1033,24 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A20" s="2">
+        <v>41884</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D20" s="3">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="1"/>
+        <v>0.8166666666666661</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1074,7 +1089,7 @@
       </c>
       <c r="E26" s="4">
         <f>SUM(E2:E25)</f>
-        <v>16.783333333333331</v>
+        <v>17.599999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on merging stuff.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -157,7 +157,11 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -165,6 +169,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hours</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -204,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.116666666666667</c:v>
+                  <c:v>11.466666666666669</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.6166666666666671</c:v>
@@ -219,7 +234,7 @@
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
-          <c:showCatName val="0"/>
+          <c:showCatName val="1"/>
           <c:showSerName val="0"/>
           <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
@@ -245,19 +260,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -565,7 +580,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +654,7 @@
       </c>
       <c r="J2" s="12">
         <f>I2/SUM($I$2:$I$5)</f>
-        <v>8.5387323943661955E-2</v>
+        <v>7.9704190632703342E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -667,11 +682,11 @@
       </c>
       <c r="I3" s="10">
         <f>SUMIF($F$2:$F$42,H3,$E$2:$E$42)</f>
-        <v>10.116666666666667</v>
+        <v>11.466666666666669</v>
       </c>
       <c r="J3" s="12">
         <f t="shared" ref="J3:J5" si="0">I3/SUM($I$2:$I$5)</f>
-        <v>0.534330985915493</v>
+        <v>0.5653245686113394</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -703,7 +718,7 @@
       </c>
       <c r="J4" s="12">
         <f t="shared" si="0"/>
-        <v>0.13820422535211269</v>
+        <v>0.12900575184880855</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -735,7 +750,7 @@
       </c>
       <c r="J5" s="12">
         <f t="shared" si="0"/>
-        <v>0.24207746478873229</v>
+        <v>0.2259654889071486</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1118,10 +1133,24 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="E24" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A24" s="2">
+        <v>41885</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.92013888888888884</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.9868055555555556</v>
+      </c>
+      <c r="D24" s="3">
+        <v>15</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="1"/>
+        <v>1.3500000000000023</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1253,7 +1282,7 @@
       </c>
       <c r="E43" s="4">
         <f>SUM(E2:E42)</f>
-        <v>18.93333333333333</v>
+        <v>20.283333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed SVG files, added background files, and converted DeviceListActivity to DeviceListFragment.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -158,7 +158,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -171,7 +170,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>Sheet2!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -191,7 +190,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$2:$H$5</c:f>
+              <c:f>Sheet2!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -211,7 +210,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$5</c:f>
+              <c:f>Sheet2!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -219,7 +218,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.766666666666669</c:v>
+                  <c:v>17.900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.45</c:v>
@@ -259,21 +258,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:rowOff>185738</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -579,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +597,7 @@
     <col min="10" max="10" width="11" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -615,17 +616,8 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>41879</v>
       </c>
@@ -645,19 +637,8 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="10">
-        <f>SUMIF($F$2:$F$42,H2,$E$2:$E$42)</f>
-        <v>1.6166666666666663</v>
-      </c>
-      <c r="J2" s="12">
-        <f>I2/SUM($I$2:$I$5)</f>
-        <v>6.3274624918460518E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>41880</v>
       </c>
@@ -677,19 +658,8 @@
       <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="10">
-        <f>SUMIF($F$2:$F$42,H3,$E$2:$E$42)</f>
-        <v>12.766666666666669</v>
-      </c>
-      <c r="J3" s="12">
-        <f t="shared" ref="J3:J5" si="0">I3/SUM($I$2:$I$5)</f>
-        <v>0.49967384213959565</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>41880</v>
       </c>
@@ -703,25 +673,14 @@
         <v>0</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E42" si="1">IF(AND(NOT(ISBLANK(B4)),NOT(ISBLANK(C4))), (C4-B4) * 24 - D4/60, "")</f>
+        <f t="shared" ref="E4:E42" si="0">IF(AND(NOT(ISBLANK(B4)),NOT(ISBLANK(C4))), (C4-B4) * 24 - D4/60, "")</f>
         <v>0.33333333333333748</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="10">
-        <f>SUMIF($F$2:$F$42,H4,$E$2:$E$42)</f>
-        <v>5.45</v>
-      </c>
-      <c r="J4" s="12">
-        <f t="shared" si="0"/>
-        <v>0.21330724070450097</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>41880</v>
       </c>
@@ -735,25 +694,14 @@
         <v>0</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.93333333333333268</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="10">
-        <f>SUMIF($F$2:$F$42,H5,$E$2:$E$42)</f>
-        <v>5.716666666666665</v>
-      </c>
-      <c r="J5" s="12">
-        <f t="shared" si="0"/>
-        <v>0.22374429223744285</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>41880</v>
       </c>
@@ -767,14 +715,14 @@
         <v>0</v>
       </c>
       <c r="E6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.0666666666666682</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>41880</v>
       </c>
@@ -788,14 +736,14 @@
         <v>0</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.53333333333333677</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>41880</v>
       </c>
@@ -809,14 +757,14 @@
         <v>10</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.91666666666666552</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>41881</v>
       </c>
@@ -830,14 +778,14 @@
         <v>5</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.63333333333333075</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>41881</v>
       </c>
@@ -851,14 +799,14 @@
         <v>15</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5999999999999988</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>41882</v>
       </c>
@@ -872,14 +820,14 @@
         <v>20</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.45</v>
       </c>
       <c r="F11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>41882</v>
       </c>
@@ -893,14 +841,14 @@
         <v>15</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.3999999999999995</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>41882</v>
       </c>
@@ -914,14 +862,14 @@
         <v>0</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1333333333333346</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>41882</v>
       </c>
@@ -935,14 +883,14 @@
         <v>0</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.56666666666666465</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>41883</v>
       </c>
@@ -956,14 +904,14 @@
         <v>5</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.36666666666666775</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>41883</v>
       </c>
@@ -977,7 +925,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.63333333333333075</v>
       </c>
       <c r="F16" t="s">
@@ -998,7 +946,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.2999999999999998</v>
       </c>
       <c r="F17" t="s">
@@ -1019,7 +967,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.6833333333333347</v>
       </c>
       <c r="F18" t="s">
@@ -1040,7 +988,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.6166666666666667</v>
       </c>
       <c r="F19" t="s">
@@ -1061,7 +1009,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.8166666666666661</v>
       </c>
       <c r="F20" t="s">
@@ -1082,7 +1030,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.26666666666666544</v>
       </c>
       <c r="F21" t="s">
@@ -1104,7 +1052,7 @@
         <v>8</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.53333333333333099</v>
       </c>
       <c r="F22" t="s">
@@ -1125,7 +1073,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.5333333333333341</v>
       </c>
       <c r="F23" t="s">
@@ -1146,7 +1094,7 @@
         <v>15</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.3500000000000023</v>
       </c>
       <c r="F24" t="s">
@@ -1167,7 +1115,7 @@
         <v>20</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.76666666666666816</v>
       </c>
       <c r="F25" t="s">
@@ -1188,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.36666666666666536</v>
       </c>
       <c r="F26" t="s">
@@ -1209,7 +1157,7 @@
         <v>10</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
       <c r="F27" t="s">
@@ -1230,7 +1178,7 @@
         <v>15</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.833333333333333</v>
       </c>
       <c r="F28" t="s">
@@ -1238,97 +1186,153 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="E29" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A29" s="2">
+        <v>41887</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.7909722222222223</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.83263888888888893</v>
+      </c>
+      <c r="D29" s="3">
+        <v>5</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91666666666666574</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="E30" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A30" s="2">
+        <v>41888</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.58611111111111114</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.66180555555555554</v>
+      </c>
+      <c r="D30" s="3">
+        <v>5</v>
+      </c>
+      <c r="E30" s="4">
+        <f t="shared" si="0"/>
+        <v>1.7333333333333323</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="E31" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A31" s="2">
+        <v>41888</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.82916666666666661</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="D31" s="3">
+        <v>10</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1833333333333338</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="E32" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A32" s="2">
+        <v>41888</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.9145833333333333</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="D32" s="3">
+        <v>25</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" si="0"/>
+        <v>1.3000000000000018</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="E33" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="E34" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="E35" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="E36" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="E37" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="E38" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="E39" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E40" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E41" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E42" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -1338,25 +1342,96 @@
       </c>
       <c r="E43" s="4">
         <f>SUM(E2:E42)</f>
-        <v>25.549999999999997</v>
+        <v>30.683333333333326</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="10">
+        <f>SUMIF(Sheet1!$F$2:$F$42,A2,Sheet1!$E$2:$E$42)</f>
+        <v>1.6166666666666663</v>
+      </c>
+      <c r="C2" s="12">
+        <f>B2/SUM($B$2:$B$5)</f>
+        <v>5.268875611080933E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="10">
+        <f>SUMIF(Sheet1!$F$2:$F$42,A3,Sheet1!$E$2:$E$42)</f>
+        <v>17.900000000000002</v>
+      </c>
+      <c r="C3" s="12">
+        <f>B3/SUM($B$2:$B$5)</f>
+        <v>0.58337859858772412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="10">
+        <f>SUMIF(Sheet1!$F$2:$F$42,A4,Sheet1!$E$2:$E$42)</f>
+        <v>5.45</v>
+      </c>
+      <c r="C4" s="12">
+        <f>B4/SUM($B$2:$B$5)</f>
+        <v>0.17762085822922324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10">
+        <f>SUMIF(Sheet1!$F$2:$F$42,A5,Sheet1!$E$2:$E$42)</f>
+        <v>5.716666666666665</v>
+      </c>
+      <c r="C5" s="12">
+        <f>B5/SUM($B$2:$B$5)</f>
+        <v>0.1863117870722433</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed BluetoothConnectionFragment and removed use of DrawerActivity.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -221,7 +221,7 @@
                   <c:v>21.250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.2833333333333359</c:v>
+                  <c:v>6.9833333333333361</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5.716666666666665</c:v>
@@ -581,7 +581,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,10 +1354,24 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="E37" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A37" s="2">
+        <v>41891</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.90555555555555556</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.93819444444444444</v>
+      </c>
+      <c r="D37" s="3">
+        <v>5</v>
+      </c>
+      <c r="E37" s="4">
+        <f t="shared" si="0"/>
+        <v>0.69999999999999984</v>
+      </c>
+      <c r="F37" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1398,7 +1412,7 @@
       </c>
       <c r="E43" s="4">
         <f>SUM(E2:E42)</f>
-        <v>34.86666666666666</v>
+        <v>35.566666666666663</v>
       </c>
     </row>
   </sheetData>
@@ -1443,7 +1457,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>4.6367112810707434E-2</v>
+        <v>4.5454545454545428E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1456,7 +1470,7 @@
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.60946462715105154</v>
+        <v>0.59746954076850978</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,11 +1479,11 @@
       </c>
       <c r="B4" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$42,A4,Sheet1!$E$2:$E$42)</f>
-        <v>6.2833333333333359</v>
+        <v>6.9833333333333361</v>
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.18021032504780118</v>
+        <v>0.1963448922211809</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1482,7 +1496,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.16395793499043967</v>
+        <v>0.16073102155576374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit changes before removing Server logic from Game.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -158,6 +158,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1375,7 +1376,12 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
+      <c r="A38" s="2">
+        <v>41892</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.53541666666666665</v>
+      </c>
       <c r="E38" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1426,7 +1432,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working on stuff still.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -158,7 +158,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -219,13 +218,13 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.250000000000004</c:v>
+                  <c:v>23.06666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6.9833333333333361</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.716666666666665</c:v>
+                  <c:v>7.2466666666666653</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -579,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E42" si="0">IF(AND(NOT(ISBLANK(B4)),NOT(ISBLANK(C4))), (C4-B4) * 24 - D4/60, "")</f>
+        <f t="shared" ref="E4:E62" si="0">IF(AND(NOT(ISBLANK(B4)),NOT(ISBLANK(C4))), (C4-B4) * 24 - D4/60, "")</f>
         <v>0.33333333333333748</v>
       </c>
       <c r="F4" t="s">
@@ -1382,43 +1381,170 @@
       <c r="B38" s="1">
         <v>0.53541666666666665</v>
       </c>
-      <c r="E38" s="4" t="str">
+      <c r="C38" s="1">
+        <v>0.56874999999999998</v>
+      </c>
+      <c r="D38" s="3">
+        <v>15</v>
+      </c>
+      <c r="E38" s="4">
+        <f t="shared" si="0"/>
+        <v>0.54999999999999982</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>41892</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.97152777777777777</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1.0227777777777778</v>
+      </c>
+      <c r="D39" s="3">
+        <v>15</v>
+      </c>
+      <c r="E39" s="4">
+        <f t="shared" si="0"/>
+        <v>0.98000000000000043</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>41893</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.45208333333333334</v>
+      </c>
+      <c r="D40" s="3">
+        <v>5</v>
+      </c>
+      <c r="E40" s="4">
+        <f t="shared" si="0"/>
+        <v>0.68333333333333324</v>
+      </c>
+      <c r="F40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>41893</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.64027777777777783</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D41" s="3">
+        <v>15</v>
+      </c>
+      <c r="E41" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1333333333333311</v>
+      </c>
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>41893</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.69861111111111107</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="F42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="E39" s="4" t="str">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E40" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E41" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E42" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="4">
-        <f>SUM(E2:E42)</f>
-        <v>35.566666666666663</v>
+      <c r="E63" s="4">
+        <f>SUM(E2:E62)</f>
+        <v>38.913333333333327</v>
       </c>
     </row>
   </sheetData>
@@ -1458,12 +1584,12 @@
         <v>6</v>
       </c>
       <c r="B2" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$42,A2,Sheet1!$E$2:$E$42)</f>
+        <f>SUMIF(Sheet1!$F$2:$F$62,A2,Sheet1!$E$2:$E$62)</f>
         <v>1.6166666666666663</v>
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>4.5454545454545428E-2</v>
+        <v>4.1545314373822161E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1471,12 +1597,12 @@
         <v>7</v>
       </c>
       <c r="B3" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$42,A3,Sheet1!$E$2:$E$42)</f>
-        <v>21.250000000000004</v>
+        <f>SUMIF(Sheet1!$F$2:$F$62,A3,Sheet1!$E$2:$E$62)</f>
+        <v>23.06666666666667</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.59746954076850978</v>
+        <v>0.59277025869453492</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1484,12 +1610,12 @@
         <v>8</v>
       </c>
       <c r="B4" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$42,A4,Sheet1!$E$2:$E$42)</f>
+        <f>SUMIF(Sheet1!$F$2:$F$62,A4,Sheet1!$E$2:$E$62)</f>
         <v>6.9833333333333361</v>
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.1963448922211809</v>
+        <v>0.17945862600651025</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1497,12 +1623,12 @@
         <v>12</v>
       </c>
       <c r="B5" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$42,A5,Sheet1!$E$2:$E$42)</f>
-        <v>5.716666666666665</v>
+        <f>SUMIF(Sheet1!$F$2:$F$62,A5,Sheet1!$E$2:$E$62)</f>
+        <v>7.2466666666666653</v>
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.16073102155576374</v>
+        <v>0.18622580092513275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes and new resources.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -221,7 +221,7 @@
                   <c:v>23.06666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.4666666666666721</c:v>
+                  <c:v>10.550000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7.2466666666666653</c:v>
@@ -581,7 +581,7 @@
   <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,10 +1480,24 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="E43" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A43" s="2">
+        <v>41897</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.8847222222222223</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0.9819444444444444</v>
+      </c>
+      <c r="D43" s="3">
+        <v>15</v>
+      </c>
+      <c r="E43" s="4">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333304</v>
+      </c>
+      <c r="F43" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1623,7 +1637,7 @@
       </c>
       <c r="E63" s="4">
         <f>SUM(E2:E62)</f>
-        <v>40.396666666666661</v>
+        <v>42.47999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1668,7 +1682,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>4.001980361415957E-2</v>
+        <v>3.8057124921531689E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1681,7 +1695,7 @@
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.57100420826800902</v>
+        <v>0.54300062774639046</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1690,11 +1704,11 @@
       </c>
       <c r="B4" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A4,Sheet1!$E$2:$E$62)</f>
-        <v>8.4666666666666721</v>
+        <v>10.550000000000002</v>
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.20958824985559876</v>
+        <v>0.24835216572504712</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1707,7 +1721,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.17938773826223281</v>
+        <v>0.17059008160703071</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enabled being able to send cards.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -218,10 +218,10 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.06666666666667</c:v>
+                  <c:v>23.983333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.550000000000002</c:v>
+                  <c:v>10.983333333333336</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7.2466666666666653</c:v>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,17 +1501,45 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="E44" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A44" s="2">
+        <v>41897</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.98333333333333339</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="D44" s="3">
+        <v>5</v>
+      </c>
+      <c r="E44" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91666666666666308</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="E45" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A45" s="2">
+        <v>41897</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2.7083333333333334E-2</v>
+      </c>
+      <c r="C45" s="1">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="D45" s="3">
+        <v>5</v>
+      </c>
+      <c r="E45" s="4">
+        <f t="shared" si="0"/>
+        <v>0.43333333333333329</v>
+      </c>
+      <c r="F45" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1637,7 +1665,7 @@
       </c>
       <c r="E63" s="4">
         <f>SUM(E2:E62)</f>
-        <v>42.47999999999999</v>
+        <v>43.829999999999984</v>
       </c>
     </row>
   </sheetData>
@@ -1682,7 +1710,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>3.8057124921531689E-2</v>
+        <v>3.6884934215529692E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1691,11 +1719,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A3,Sheet1!$E$2:$E$62)</f>
-        <v>23.06666666666667</v>
+        <v>23.983333333333334</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.54300062774639046</v>
+        <v>0.54718990037265192</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1704,11 +1732,11 @@
       </c>
       <c r="B4" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A4,Sheet1!$E$2:$E$62)</f>
-        <v>10.550000000000002</v>
+        <v>10.983333333333336</v>
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.24835216572504712</v>
+        <v>0.25058939843334099</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1721,7 +1749,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.17059008160703071</v>
+        <v>0.16533576697847743</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issues with CardDrawable.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -114,7 +114,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -128,6 +128,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -218,10 +219,10 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.983333333333334</c:v>
+                  <c:v>25.116666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.983333333333336</c:v>
+                  <c:v>13.216666666666669</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7.2466666666666653</c:v>
@@ -580,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,7 +1524,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>41897</v>
+        <v>41898</v>
       </c>
       <c r="B45" s="1">
         <v>2.7083333333333334E-2</v>
@@ -1543,129 +1544,185 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="E46" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A46" s="2">
+        <v>41898</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.45208333333333334</v>
+      </c>
+      <c r="D46" s="3">
+        <v>5</v>
+      </c>
+      <c r="E46" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1666666666666676</v>
+      </c>
+      <c r="F46" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="E47" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A47" s="2">
+        <v>41898</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.72083333333333333</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.75486111111111109</v>
+      </c>
+      <c r="D47" s="3">
+        <v>20</v>
+      </c>
+      <c r="E47" s="4">
+        <f t="shared" si="0"/>
+        <v>0.48333333333333311</v>
+      </c>
+      <c r="F47" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="E48" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="E49" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>41898</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.97569444444444453</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1.0368055555555555</v>
+      </c>
+      <c r="D48" s="3">
+        <v>20</v>
+      </c>
+      <c r="E48" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1333333333333309</v>
+      </c>
+      <c r="F48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>41899</v>
+      </c>
+      <c r="B49" s="13">
+        <v>0.57777777777777783</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.6020833333333333</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="E49" s="4">
+        <f t="shared" si="0"/>
+        <v>0.58333333333333126</v>
+      </c>
+      <c r="F49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="E50" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="E51" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="E52" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="E53" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="E54" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="E55" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="E56" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="E57" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="E58" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="E59" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="E60" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E61" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E62" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>9</v>
       </c>
       <c r="E63" s="4">
         <f>SUM(E2:E62)</f>
-        <v>43.829999999999984</v>
+        <v>47.196666666666644</v>
       </c>
     </row>
   </sheetData>
@@ -1710,7 +1767,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>3.6884934215529692E-2</v>
+        <v>3.4253831485274375E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1719,11 +1776,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A3,Sheet1!$E$2:$E$62)</f>
-        <v>23.983333333333334</v>
+        <v>25.116666666666664</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.54718990037265192</v>
+        <v>0.53217035101348964</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1732,11 +1789,11 @@
       </c>
       <c r="B4" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A4,Sheet1!$E$2:$E$62)</f>
-        <v>10.983333333333336</v>
+        <v>13.216666666666669</v>
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.25058939843334099</v>
+        <v>0.28003390069920198</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1749,7 +1806,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.16533576697847743</v>
+        <v>0.15354191680203402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extracted GameGestureListener out of GameView. Added Crashlytics.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.116666666666664</c:v>
+                  <c:v>25.383333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>13.216666666666669</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,10 +1628,24 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="E50" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A50" s="2">
+        <v>41899</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.60347222222222219</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0</v>
+      </c>
+      <c r="E50" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26666666666666838</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1722,7 +1736,7 @@
       </c>
       <c r="E63" s="4">
         <f>SUM(E2:E62)</f>
-        <v>47.196666666666644</v>
+        <v>47.46333333333331</v>
       </c>
     </row>
   </sheetData>
@@ -1767,7 +1781,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>3.4253831485274375E-2</v>
+        <v>3.406138071493784E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1776,11 +1790,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A3,Sheet1!$E$2:$E$62)</f>
-        <v>25.116666666666664</v>
+        <v>25.383333333333333</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.53217035101348964</v>
+        <v>0.53479879205000358</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1793,7 +1807,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.28003390069920198</v>
+        <v>0.27846056605098679</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1806,7 +1820,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.15354191680203402</v>
+        <v>0.15267926118407188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added DeckSettings. Fixed issues with Player names.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -222,7 +222,7 @@
                   <c:v>25.383333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.216666666666669</c:v>
+                  <c:v>16.95</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7.2466666666666653</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,17 +1649,45 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="E51" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A51" s="2">
+        <v>41899</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1.0506944444444444</v>
+      </c>
+      <c r="D51" s="3">
+        <v>20</v>
+      </c>
+      <c r="E51" s="4">
+        <f t="shared" si="0"/>
+        <v>2.0499999999999994</v>
+      </c>
+      <c r="F51" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="E52" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A52" s="2">
+        <v>41900</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.69930555555555562</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.78333333333333333</v>
+      </c>
+      <c r="D52" s="3">
+        <v>20</v>
+      </c>
+      <c r="E52" s="4">
+        <f t="shared" si="0"/>
+        <v>1.6833333333333316</v>
+      </c>
+      <c r="F52" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1736,7 +1764,7 @@
       </c>
       <c r="E63" s="4">
         <f>SUM(E2:E62)</f>
-        <v>47.46333333333331</v>
+        <v>51.196666666666637</v>
       </c>
     </row>
   </sheetData>
@@ -1781,7 +1809,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>3.406138071493784E-2</v>
+        <v>3.1577576665147461E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1794,7 +1822,7 @@
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.53479879205000358</v>
+        <v>0.49580050784556284</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1803,11 +1831,11 @@
       </c>
       <c r="B4" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A4,Sheet1!$E$2:$E$62)</f>
-        <v>13.216666666666669</v>
+        <v>16.95</v>
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.27846056605098679</v>
+        <v>0.3310762419428348</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1820,7 +1848,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.15267926118407188</v>
+        <v>0.14154567354645484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-fixed sending of player name to server.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,10 +219,10 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.383333333333333</c:v>
+                  <c:v>25.966666666666665</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.95</c:v>
+                  <c:v>18.016666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7.2466666666666653</c:v>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,17 +1691,45 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="E53" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A53" s="2">
+        <v>41901</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D53" s="3">
+        <v>10</v>
+      </c>
+      <c r="E53" s="4">
+        <f t="shared" si="0"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-      <c r="E54" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A54" s="2">
+        <v>41901</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.9784722222222223</v>
+      </c>
+      <c r="D54" s="3">
+        <v>10</v>
+      </c>
+      <c r="E54" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0666666666666675</v>
+      </c>
+      <c r="F54" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1764,7 +1792,7 @@
       </c>
       <c r="E63" s="4">
         <f>SUM(E2:E62)</f>
-        <v>51.196666666666637</v>
+        <v>52.846666666666643</v>
       </c>
     </row>
   </sheetData>
@@ -1809,7 +1837,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>3.1577576665147461E-2</v>
+        <v>3.0591648795256714E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1818,11 +1846,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A3,Sheet1!$E$2:$E$62)</f>
-        <v>25.383333333333333</v>
+        <v>25.966666666666665</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.49580050784556284</v>
+        <v>0.49135864765989662</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1831,11 +1859,11 @@
       </c>
       <c r="B4" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A4,Sheet1!$E$2:$E$62)</f>
-        <v>16.95</v>
+        <v>18.016666666666666</v>
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.3310762419428348</v>
+        <v>0.3409234262646651</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1848,7 +1876,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.14154567354645484</v>
+        <v>0.13712627728018165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Game background preference.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.966666666666665</c:v>
+                  <c:v>26.349999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>18.016666666666666</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,14 +1733,33 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
-      <c r="E55" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A55" s="2">
+        <v>41901</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.97986111111111107</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1.0027777777777778</v>
+      </c>
+      <c r="D55" s="3">
+        <v>10</v>
+      </c>
+      <c r="E55" s="4">
+        <f t="shared" si="0"/>
+        <v>0.38333333333333408</v>
+      </c>
+      <c r="F55" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
+      <c r="A56" s="2">
+        <v>41902</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="E56" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1792,7 +1811,7 @@
       </c>
       <c r="E63" s="4">
         <f>SUM(E2:E62)</f>
-        <v>52.846666666666643</v>
+        <v>53.229999999999976</v>
       </c>
     </row>
   </sheetData>
@@ -1837,7 +1856,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>3.0591648795256714E-2</v>
+        <v>3.0371344479929858E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1846,11 +1865,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A3,Sheet1!$E$2:$E$62)</f>
-        <v>25.966666666666665</v>
+        <v>26.349999999999998</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.49135864765989662</v>
+        <v>0.4950216043584445</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1863,7 +1882,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.3409234262646651</v>
+        <v>0.33846828229695036</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1876,7 +1895,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.13712627728018165</v>
+        <v>0.1361387688646753</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ability to layout cards by suit and rank.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,10 +219,10 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.349999999999998</c:v>
+                  <c:v>26.68333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.016666666666666</c:v>
+                  <c:v>19.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7.2466666666666653</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,16 +1760,39 @@
       <c r="B56" s="1">
         <v>0.73958333333333337</v>
       </c>
-      <c r="E56" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="C56" s="1">
+        <v>0.83472222222222225</v>
+      </c>
+      <c r="D56" s="3">
+        <v>30</v>
+      </c>
+      <c r="E56" s="4">
+        <f t="shared" si="0"/>
+        <v>1.7833333333333332</v>
+      </c>
+      <c r="F56" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="E57" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A57" s="2">
+        <v>41902</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0.97361111111111109</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0.98749999999999993</v>
+      </c>
+      <c r="D57" s="3">
+        <v>0</v>
+      </c>
+      <c r="E57" s="4">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333215</v>
+      </c>
+      <c r="F57" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1811,7 +1834,7 @@
       </c>
       <c r="E63" s="4">
         <f>SUM(E2:E62)</f>
-        <v>53.229999999999976</v>
+        <v>55.346666666666636</v>
       </c>
     </row>
   </sheetData>
@@ -1856,7 +1879,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>3.0371344479929858E-2</v>
+        <v>2.9209828956877858E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1865,11 +1888,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A3,Sheet1!$E$2:$E$62)</f>
-        <v>26.349999999999998</v>
+        <v>26.68333333333333</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.4950216043584445</v>
+        <v>0.48211274391712844</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1878,11 +1901,11 @@
       </c>
       <c r="B4" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A4,Sheet1!$E$2:$E$62)</f>
-        <v>18.016666666666666</v>
+        <v>19.799999999999997</v>
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.33846828229695036</v>
+        <v>0.35774512165743194</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1895,7 +1918,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.1361387688646753</v>
+        <v>0.1309323054685618</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on getting saving to work correctly.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.68333333333333</c:v>
+                  <c:v>33.216666666666661</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,24 +1796,66 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="E58" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A58" s="2">
+        <v>41903</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1.0138888888888888</v>
+      </c>
+      <c r="D58" s="3">
+        <v>20</v>
+      </c>
+      <c r="E58" s="4">
+        <f t="shared" si="0"/>
+        <v>2.9999999999999987</v>
+      </c>
+      <c r="F58" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="E59" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A59" s="2">
+        <v>41904</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0.53611111111111109</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0.61319444444444449</v>
+      </c>
+      <c r="D59" s="3">
+        <v>10</v>
+      </c>
+      <c r="E59" s="4">
+        <f t="shared" si="0"/>
+        <v>1.6833333333333347</v>
+      </c>
+      <c r="F59" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
-      <c r="E60" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A60" s="2">
+        <v>41904</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1.0770833333333334</v>
+      </c>
+      <c r="D60" s="3">
+        <v>15</v>
+      </c>
+      <c r="E60" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8500000000000005</v>
+      </c>
+      <c r="F60" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1834,7 +1876,7 @@
       </c>
       <c r="E63" s="4">
         <f>SUM(E2:E62)</f>
-        <v>55.346666666666636</v>
+        <v>61.879999999999974</v>
       </c>
     </row>
   </sheetData>
@@ -1879,7 +1921,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>2.9209828956877858E-2</v>
+        <v>2.6125834949364359E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1888,11 +1930,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$62,A3,Sheet1!$E$2:$E$62)</f>
-        <v>26.68333333333333</v>
+        <v>33.216666666666661</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.48211274391712844</v>
+        <v>0.53679163973281618</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1905,7 +1947,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.35774512165743194</v>
+        <v>0.3199741435035553</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1918,7 +1960,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.1309323054685618</v>
+        <v>0.11710838181426417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ability to save games.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.566666666666656</c:v>
+                  <c:v>35.133333333333319</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,7 +1880,25 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
+      <c r="A62" s="2">
+        <v>41905</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1.0270833333333333</v>
+      </c>
+      <c r="D62" s="3">
+        <v>5</v>
+      </c>
+      <c r="E62" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5666666666666662</v>
+      </c>
+      <c r="F62" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
@@ -1954,7 +1972,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>62.229999999999968</v>
+        <v>63.796666666666631</v>
       </c>
     </row>
   </sheetData>
@@ -1999,7 +2017,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>2.5978895495205958E-2</v>
+        <v>2.5340926903181987E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2008,11 +2026,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>33.566666666666656</v>
+        <v>35.133333333333319</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.53939686110664731</v>
+        <v>0.55070797847327446</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2025,7 +2043,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.31817451390004825</v>
+        <v>0.31036104289670313</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2038,7 +2056,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.11644972949809847</v>
+        <v>0.1135900517268405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adapting current implementation to work with a table view for discard/draw card piles.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -159,6 +159,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -219,7 +220,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.133333333333319</c:v>
+                  <c:v>36.083333333333314</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -581,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1901,58 +1902,144 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
+      <c r="A63" s="2">
+        <v>41907</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0.85625000000000007</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="D63" s="3">
+        <v>20</v>
+      </c>
+      <c r="E63" s="4">
+        <f t="shared" si="0"/>
+        <v>0.94999999999999818</v>
+      </c>
+      <c r="F63" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E64" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E65" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E66" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E67" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E68" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E69" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E70" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E71" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E72" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E73" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E74" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E75" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E76" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E77" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E78" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E79" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
+      <c r="E80" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E81" s="4" t="str">
@@ -1972,7 +2059,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>63.796666666666631</v>
+        <v>64.746666666666627</v>
       </c>
     </row>
   </sheetData>
@@ -1986,7 +2073,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2017,7 +2104,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>2.5340926903181987E-2</v>
+        <v>2.4969110378912689E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2026,11 +2113,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>35.133333333333319</v>
+        <v>36.083333333333314</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.55070797847327446</v>
+        <v>0.55730024711696857</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2043,7 +2130,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.31036104289670313</v>
+        <v>0.30580724876441523</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2056,7 +2143,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.1135900517268405</v>
+        <v>0.11192339373970348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Making changes to allow multiple GameConnectionListeners to add TableView feature.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -159,7 +159,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -220,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.083333333333314</c:v>
+                  <c:v>38.649999999999977</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,118 +1922,160 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-      <c r="E64" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="E65" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="E66" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>41908</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0.73055555555555562</v>
+      </c>
+      <c r="D64" s="3">
+        <v>10</v>
+      </c>
+      <c r="E64" s="4">
+        <f t="shared" si="0"/>
+        <v>0.61666666666666925</v>
+      </c>
+      <c r="F64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>41909</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0.63611111111111118</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0.67847222222222225</v>
+      </c>
+      <c r="D65" s="3">
+        <v>5</v>
+      </c>
+      <c r="E65" s="4">
+        <f t="shared" si="0"/>
+        <v>0.93333333333333235</v>
+      </c>
+      <c r="F65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>41910</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0.94652777777777775</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="D66" s="3">
+        <v>15</v>
+      </c>
+      <c r="E66" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0166666666666675</v>
+      </c>
+      <c r="F66" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="E67" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="E68" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="E69" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="E70" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="E71" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="E72" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="E73" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="E74" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="E75" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="E76" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="E77" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="E78" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="E79" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="E80" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2059,7 +2100,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>64.746666666666627</v>
+        <v>67.313333333333304</v>
       </c>
     </row>
   </sheetData>
@@ -2104,7 +2145,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>2.4969110378912689E-2</v>
+        <v>2.4017034762800836E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2113,11 +2154,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>36.083333333333314</v>
+        <v>38.649999999999977</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.55730024711696857</v>
+        <v>0.57418044963850645</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2130,7 +2171,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.30580724876441523</v>
+        <v>0.29414677627017932</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2143,7 +2184,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.11192339373970348</v>
+        <v>0.10765573932851344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added custom Deck launcher icon.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.699999999999974</c:v>
+                  <c:v>39.816666666666642</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,10 +2006,24 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
-      <c r="E68" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A68" s="2">
+        <v>41911</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0.92638888888888893</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0.93125000000000002</v>
+      </c>
+      <c r="D68" s="3">
+        <v>0</v>
+      </c>
+      <c r="E68" s="4">
+        <f t="shared" si="0"/>
+        <v>0.11666666666666625</v>
+      </c>
+      <c r="F68" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2114,7 +2128,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>68.363333333333301</v>
+        <v>68.479999999999961</v>
       </c>
     </row>
   </sheetData>
@@ -2159,7 +2173,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>2.3648154468769812E-2</v>
+        <v>2.3607866043613708E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2168,11 +2182,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>39.699999999999974</v>
+        <v>39.816666666666642</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.58072065922278016</v>
+        <v>0.58143496884735191</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2185,7 +2199,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.28962894339070661</v>
+        <v>0.28913551401869164</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2198,7 +2212,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.10600224291774346</v>
+        <v>0.10582165109034269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed unneeded compatibility libraries.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.816666666666642</c:v>
+                  <c:v>41.549999999999976</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,10 +2027,24 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="2"/>
-      <c r="E69" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A69" s="2">
+        <v>41912</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0.8569444444444444</v>
+      </c>
+      <c r="D69" s="3">
+        <v>20</v>
+      </c>
+      <c r="E69" s="4">
+        <f t="shared" si="0"/>
+        <v>1.7333333333333314</v>
+      </c>
+      <c r="F69" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2128,7 +2142,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>68.479999999999961</v>
+        <v>70.213333333333296</v>
       </c>
     </row>
   </sheetData>
@@ -2173,7 +2187,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>2.3607866043613708E-2</v>
+        <v>2.3025066464109383E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2182,11 +2196,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>39.816666666666642</v>
+        <v>41.549999999999976</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.58143496884735191</v>
+        <v>0.59176794530953269</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2199,7 +2213,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.28913551401869164</v>
+        <v>0.28199772123053557</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2212,7 +2226,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.10582165109034269</v>
+        <v>0.10320926699582227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on implementing TableView.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.549999999999976</c:v>
+                  <c:v>46.499999999999979</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,17 +2048,45 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="2"/>
-      <c r="E70" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A70" s="2">
+        <v>41913</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C70" s="1">
+        <v>0.57777777777777783</v>
+      </c>
+      <c r="D70" s="3">
+        <v>15</v>
+      </c>
+      <c r="E70" s="4">
+        <f t="shared" si="0"/>
+        <v>0.95000000000000107</v>
+      </c>
+      <c r="F70" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
-      <c r="E71" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A71" s="2">
+        <v>41913</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0.8881944444444444</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1.0756944444444445</v>
+      </c>
+      <c r="D71" s="3">
+        <v>30</v>
+      </c>
+      <c r="E71" s="4">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000027</v>
+      </c>
+      <c r="F71" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2142,7 +2170,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>70.213333333333296</v>
+        <v>75.163333333333298</v>
       </c>
     </row>
   </sheetData>
@@ -2187,7 +2215,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>2.3025066464109383E-2</v>
+        <v>2.1508714355403788E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2196,11 +2224,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>41.549999999999976</v>
+        <v>46.499999999999979</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.59176794530953269</v>
+        <v>0.61865271187192328</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2213,7 +2241,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.28199772123053557</v>
+        <v>0.26342631602288352</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2226,7 +2254,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>0.10320926699582227</v>
+        <v>9.6412257749789357E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issues with sending and removing cards from Table. Still have issue with cards being added too many times to virtual representation of game.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.499999999999979</c:v>
+                  <c:v>47.616666666666646</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2090,10 +2090,24 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="2"/>
-      <c r="E72" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A72" s="2">
+        <v>41916</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1.01875</v>
+      </c>
+      <c r="D72" s="3">
+        <v>20</v>
+      </c>
+      <c r="E72" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1166666666666669</v>
+      </c>
+      <c r="F72" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2170,7 +2184,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>75.163333333333298</v>
+        <v>76.279999999999959</v>
       </c>
     </row>
   </sheetData>
@@ -2215,7 +2229,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>2.1508714355403788E-2</v>
+        <v>2.1193847229505333E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2224,11 +2238,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>46.499999999999979</v>
+        <v>47.616666666666646</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.61865271187192328</v>
+        <v>0.62423527355357455</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2241,7 +2255,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.26342631602288352</v>
+        <v>0.25957000524383855</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2254,7 +2268,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>9.6412257749789357E-2</v>
+        <v>9.5000873973081643E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on fixing issues with sending cards to Table.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47.616666666666646</c:v>
+                  <c:v>48.749999999999979</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,17 +2111,45 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
-      <c r="E73" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A73" s="2">
+        <v>41917</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.95763888888888893</v>
+      </c>
+      <c r="C73" s="1">
+        <v>0.98263888888888884</v>
+      </c>
+      <c r="D73" s="3">
+        <v>5</v>
+      </c>
+      <c r="E73" s="4">
+        <f t="shared" si="0"/>
+        <v>0.5166666666666645</v>
+      </c>
+      <c r="F73" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="2"/>
-      <c r="E74" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A74" s="2">
+        <v>41918</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0.59166666666666667</v>
+      </c>
+      <c r="D74" s="3">
+        <v>15</v>
+      </c>
+      <c r="E74" s="4">
+        <f t="shared" si="0"/>
+        <v>0.61666666666666625</v>
+      </c>
+      <c r="F74" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2184,7 +2212,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>76.279999999999959</v>
+        <v>77.413333333333284</v>
       </c>
     </row>
   </sheetData>
@@ -2229,7 +2257,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>2.1193847229505333E-2</v>
+        <v>2.0883568722011712E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2238,11 +2266,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>47.616666666666646</v>
+        <v>48.749999999999979</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.62423527355357455</v>
+        <v>0.62973647950396128</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2255,7 +2283,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.25957000524383855</v>
+        <v>0.25576989321391669</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2268,7 +2296,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>9.5000873973081643E-2</v>
+        <v>9.3610058560110232E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
State of game is now fixed.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.749999999999979</c:v>
+                  <c:v>49.233333333333313</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2153,10 +2153,24 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="2"/>
-      <c r="E75" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A75" s="2">
+        <v>41918</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="C75" s="1">
+        <v>0.61736111111111114</v>
+      </c>
+      <c r="D75" s="3">
+        <v>5</v>
+      </c>
+      <c r="E75" s="4">
+        <f t="shared" si="0"/>
+        <v>0.483333333333334</v>
+      </c>
+      <c r="F75" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2212,7 +2226,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>77.413333333333284</v>
+        <v>77.896666666666619</v>
       </c>
     </row>
   </sheetData>
@@ -2257,7 +2271,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>2.0883568722011712E-2</v>
+        <v>2.0753990329068425E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2266,11 +2280,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>48.749999999999979</v>
+        <v>49.233333333333313</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.62973647950396128</v>
+        <v>0.63203389105224861</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2283,7 +2297,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.25576989321391669</v>
+        <v>0.25418289186529164</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2296,7 +2310,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>9.3610058560110232E-2</v>
+        <v>9.3029226753391245E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished implementing TableView. Refining of features still required.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.233333333333313</c:v>
+                  <c:v>53.59999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2174,10 +2174,24 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
-      <c r="E76" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A76" s="2">
+        <v>41918</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0.93125000000000002</v>
+      </c>
+      <c r="C76" s="1">
+        <v>1.1340277777777779</v>
+      </c>
+      <c r="D76" s="3">
+        <v>30</v>
+      </c>
+      <c r="E76" s="4">
+        <f t="shared" si="0"/>
+        <v>4.366666666666668</v>
+      </c>
+      <c r="F76" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2226,7 +2240,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>77.896666666666619</v>
+        <v>82.263333333333293</v>
       </c>
     </row>
   </sheetData>
@@ -2271,7 +2285,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>2.0753990329068425E-2</v>
+        <v>1.9652335994165077E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2280,11 +2294,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>49.233333333333313</v>
+        <v>53.59999999999998</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.63203389105224861</v>
+        <v>0.65156610883747301</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2297,7 +2311,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.25418289186529164</v>
+        <v>0.24069046557802179</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2310,7 +2324,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>9.3029226753391245E-2</v>
+        <v>8.8091089590339955E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added .idea folder to .gitignore. Fixed actionbar overlaying content.
Fixes #6
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -2195,7 +2195,12 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="2"/>
+      <c r="A77" s="2">
+        <v>41919</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0.73125000000000007</v>
+      </c>
       <c r="E77" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
Made TableView un-draggable. Added vibration when a card is received.
Closes #4
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.59999999999998</c:v>
+                  <c:v>54.549999999999976</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,9 +2201,18 @@
       <c r="B77" s="1">
         <v>0.73125000000000007</v>
       </c>
-      <c r="E77" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="C77" s="1">
+        <v>0.78125</v>
+      </c>
+      <c r="D77" s="3">
+        <v>15</v>
+      </c>
+      <c r="E77" s="4">
+        <f t="shared" si="0"/>
+        <v>0.9499999999999984</v>
+      </c>
+      <c r="F77" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2245,7 +2254,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>82.263333333333293</v>
+        <v>83.213333333333296</v>
       </c>
     </row>
   </sheetData>
@@ -2290,7 +2299,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.9652335994165077E-2</v>
+        <v>1.9427976285851627E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2299,11 +2308,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>53.59999999999998</v>
+        <v>54.549999999999976</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.65156610883747301</v>
+        <v>0.65554398333600372</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2316,7 +2325,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.24069046557802179</v>
+        <v>0.23794263739785293</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2329,7 +2338,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>8.8091089590339955E-2</v>
+        <v>8.7085402980291632E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Have TableView working with moveable cards.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.549999999999976</c:v>
+                  <c:v>55.46666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2216,10 +2216,24 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-      <c r="E78" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A78" s="2">
+        <v>41919</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0.96527777777777779</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1.0173611111111112</v>
+      </c>
+      <c r="D78" s="3">
+        <v>20</v>
+      </c>
+      <c r="E78" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91666666666666763</v>
+      </c>
+      <c r="F78" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2254,7 +2268,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>83.213333333333296</v>
+        <v>84.129999999999967</v>
       </c>
     </row>
   </sheetData>
@@ -2299,7 +2313,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.9427976285851627E-2</v>
+        <v>1.9216292246127028E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2308,11 +2322,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>54.549999999999976</v>
+        <v>55.46666666666664</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.65554398333600372</v>
+        <v>0.65929711953722403</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2325,7 +2339,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.23794263739785293</v>
+        <v>0.23535005348864857</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2338,7 +2352,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>8.7085402980291632E-2</v>
+        <v>8.6136534728000327E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switched from AndroidSlidingUpPanel to custom SlidingFrameLayout. Working on adding shadow to TableView.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.46666666666664</c:v>
+                  <c:v>57.416666666666643</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2237,10 +2237,24 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="E79" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A79" s="2">
+        <v>41920</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0.5229166666666667</v>
+      </c>
+      <c r="C79" s="1">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D79" s="3">
+        <v>15</v>
+      </c>
+      <c r="E79" s="4">
+        <f t="shared" si="0"/>
+        <v>1.9500000000000002</v>
+      </c>
+      <c r="F79" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2268,7 +2282,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>84.129999999999967</v>
+        <v>86.07999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2313,7 +2327,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.9216292246127028E-2</v>
+        <v>1.878097893432466E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2322,11 +2336,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>55.46666666666664</v>
+        <v>57.416666666666643</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.65929711953722403</v>
+        <v>0.66701517967781898</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2339,7 +2353,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.23535005348864857</v>
+        <v>0.2300185873605948</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2352,7 +2366,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>8.6136534728000327E-2</v>
+        <v>8.4185254027261458E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed card being able to be removed from Table at two devices at the same time.
Fixes #13
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57.416666666666643</c:v>
+                  <c:v>58.949999999999974</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2258,10 +2258,24 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="E80" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A80" s="2">
+        <v>41921</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0.8881944444444444</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="D80" s="3">
+        <v>15</v>
+      </c>
+      <c r="E80" s="4">
+        <f t="shared" si="0"/>
+        <v>1.533333333333335</v>
+      </c>
+      <c r="F80" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2282,7 +2296,7 @@
       </c>
       <c r="E83" s="4">
         <f>SUM(E2:E82)</f>
-        <v>86.07999999999997</v>
+        <v>87.613333333333301</v>
       </c>
     </row>
   </sheetData>
@@ -2327,7 +2341,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.878097893432466E-2</v>
+        <v>1.845229036676305E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2336,11 +2350,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
-        <v>57.416666666666643</v>
+        <v>58.949999999999974</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.66701517967781898</v>
+        <v>0.67284279409526693</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2353,7 +2367,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.2300185873605948</v>
+        <v>0.22599299954344851</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2366,7 +2380,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>8.4185254027261458E-2</v>
+        <v>8.2711915994521379E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ability to Fling TableView closed.
Closes #10
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -579,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E82" si="0">IF(AND(NOT(ISBLANK(B4)),NOT(ISBLANK(C4))), (C4-B4) * 24 - D4/60, "")</f>
+        <f t="shared" ref="E4:E103" si="0">IF(AND(NOT(ISBLANK(B4)),NOT(ISBLANK(C4))), (C4-B4) * 24 - D4/60, "")</f>
         <v>0.33333333333333748</v>
       </c>
       <c r="F4" t="s">
@@ -2279,23 +2279,92 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>41923</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0.43541666666666662</v>
+      </c>
       <c r="E81" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="4" t="str">
+      <c r="A82" s="2"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="2"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="2"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="2"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="2"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="2"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="2"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="2"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E103" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>9</v>
       </c>
-      <c r="E83" s="4">
-        <f>SUM(E2:E82)</f>
+      <c r="E104" s="4">
+        <f>SUM(E2:E103)</f>
         <v>87.613333333333301</v>
       </c>
     </row>
@@ -2336,7 +2405,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$82,A2,Sheet1!$E$2:$E$82)</f>
+        <f>SUMIF(Sheet1!$F$2:$F$103,A2,Sheet1!$E$2:$E$103)</f>
         <v>1.6166666666666663</v>
       </c>
       <c r="C2" s="12">
@@ -2349,7 +2418,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$82,A3,Sheet1!$E$2:$E$82)</f>
+        <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
         <v>58.949999999999974</v>
       </c>
       <c r="C3" s="12">
@@ -2362,7 +2431,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$82,A4,Sheet1!$E$2:$E$82)</f>
+        <f>SUMIF(Sheet1!$F$2:$F$103,A4,Sheet1!$E$2:$E$103)</f>
         <v>19.799999999999997</v>
       </c>
       <c r="C4" s="12">
@@ -2375,7 +2444,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$82,A5,Sheet1!$E$2:$E$82)</f>
+        <f>SUMIF(Sheet1!$F$2:$F$103,A5,Sheet1!$E$2:$E$103)</f>
         <v>7.2466666666666653</v>
       </c>
       <c r="C5" s="12">

</xml_diff>

<commit_message>
Improved GameSave selection list with player names.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58.949999999999974</c:v>
+                  <c:v>61.166666666666643</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,61 +2278,70 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>41923</v>
       </c>
       <c r="B81" s="1">
-        <v>0.43541666666666662</v>
-      </c>
-      <c r="E81" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.59305555555555556</v>
+      </c>
+      <c r="C81" s="1">
+        <v>0.70624999999999993</v>
+      </c>
+      <c r="D81" s="3">
+        <v>30</v>
+      </c>
+      <c r="E81" s="4">
+        <f t="shared" si="0"/>
+        <v>2.216666666666665</v>
+      </c>
+      <c r="F81" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2365,7 +2374,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>87.613333333333301</v>
+        <v>89.82999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2410,7 +2419,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.845229036676305E-2</v>
+        <v>1.7996957215481092E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2419,11 +2428,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>58.949999999999974</v>
+        <v>61.166666666666643</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.67284279409526693</v>
+        <v>0.68091580392593398</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2436,7 +2445,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.22599299954344851</v>
+        <v>0.22041634197929422</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2449,7 +2458,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>8.2711915994521379E-2</v>
+        <v>8.0670896879290507E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switched to using Croutons instead of Toasts.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>61.166666666666643</c:v>
+                  <c:v>63.049999999999976</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,7 +2300,25 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
+      <c r="A82" s="2">
+        <v>41924</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="C82" s="1">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="D82" s="3">
+        <v>60</v>
+      </c>
+      <c r="E82" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8833333333333337</v>
+      </c>
+      <c r="F82" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
@@ -2374,7 +2392,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>89.82999999999997</v>
+        <v>91.71333333333331</v>
       </c>
     </row>
   </sheetData>
@@ -2419,7 +2437,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.7996957215481092E-2</v>
+        <v>1.762738969252017E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2428,11 +2446,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>61.166666666666643</v>
+        <v>63.049999999999976</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.68091580392593398</v>
+        <v>0.68746819800828662</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2445,7 +2463,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.22041634197929422</v>
+        <v>0.21589009231663883</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2458,7 +2476,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>8.0670896879290507E-2</v>
+        <v>7.9014319982554343E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issues with how players connect to game.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.049999999999976</c:v>
+                  <c:v>63.916666666666643</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,64 +2321,158 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
+      <c r="A83" s="2">
+        <v>41924</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="C83" s="1">
+        <v>0.87638888888888899</v>
+      </c>
+      <c r="D83" s="3">
+        <v>20</v>
+      </c>
+      <c r="E83" s="4">
+        <f t="shared" si="0"/>
+        <v>0.86666666666667047</v>
+      </c>
+      <c r="F83" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
+      <c r="E84" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
+      <c r="E85" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
+      <c r="E86" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
+      <c r="E87" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
+      <c r="E88" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
+      <c r="E89" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
+      <c r="E90" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
+      <c r="E91" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
+      <c r="E92" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
+      <c r="E93" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
+      <c r="E94" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
+      <c r="E95" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
+      <c r="E96" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
+      <c r="E97" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
+      <c r="E98" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
+      <c r="E99" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
+      <c r="E100" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
+      <c r="E101" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
+      <c r="E102" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E103" s="4" t="str">
@@ -2392,7 +2486,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>91.71333333333331</v>
+        <v>92.579999999999984</v>
       </c>
     </row>
   </sheetData>
@@ -2437,7 +2531,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.762738969252017E-2</v>
+        <v>1.7462374882984088E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2446,11 +2540,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>63.049999999999976</v>
+        <v>63.916666666666643</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.68746819800828662</v>
+        <v>0.69039389356952541</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2463,7 +2557,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.21589009231663883</v>
+        <v>0.21386908619572265</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2476,7 +2570,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>7.9014319982554343E-2</v>
+        <v>7.8274645351767855E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Scan button in DevicesListActivity to ActionProcessButton.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.916666666666643</c:v>
+                  <c:v>65.46666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,10 +2342,24 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="2"/>
-      <c r="E84" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A84" s="2">
+        <v>41955</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0.87708333333333333</v>
+      </c>
+      <c r="C84" s="1">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="D84" s="3">
+        <v>30</v>
+      </c>
+      <c r="E84" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5500000000000007</v>
+      </c>
+      <c r="F84" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2486,7 +2500,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>92.579999999999984</v>
+        <v>94.129999999999981</v>
       </c>
     </row>
   </sheetData>
@@ -2531,7 +2545,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.7462374882984088E-2</v>
+        <v>1.7174829137009101E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2540,11 +2554,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>63.916666666666643</v>
+        <v>65.46666666666664</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.69039389356952541</v>
+        <v>0.69549205000177061</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2557,7 +2571,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.21386908619572265</v>
+        <v>0.21034739190481253</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2570,7 +2584,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>7.8274645351767855E-2</v>
+        <v>7.6985728956407817E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issue with drawing bitmap being too small when phone turned to landscape view.
Fixes #18
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65.46666666666664</c:v>
+                  <c:v>65.8333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2363,10 +2363,24 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="2"/>
-      <c r="E85" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A85" s="2">
+        <v>41926</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0.38125000000000003</v>
+      </c>
+      <c r="C85" s="1">
+        <v>0.39652777777777781</v>
+      </c>
+      <c r="D85" s="3">
+        <v>0</v>
+      </c>
+      <c r="E85" s="4">
+        <f t="shared" si="0"/>
+        <v>0.3666666666666667</v>
+      </c>
+      <c r="F85" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2500,7 +2514,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>94.129999999999981</v>
+        <v>94.496666666666641</v>
       </c>
     </row>
   </sheetData>
@@ -2545,7 +2559,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.7174829137009101E-2</v>
+        <v>1.7108187237645071E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2554,11 +2568,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>65.46666666666664</v>
+        <v>65.8333333333333</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.69549205000177061</v>
+        <v>0.69667360400719591</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2571,7 +2585,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.21034739190481253</v>
+        <v>0.20953120039507572</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2584,7 +2598,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>7.6985728956407817E-2</v>
+        <v>7.668700836008327E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed DrawerLayout not closing when Back was pressed.
Fixes #17
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2384,10 +2384,18 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="2"/>
-      <c r="E86" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A86" s="2">
+        <v>41926</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="C86" s="1">
+        <v>0.42638888888888887</v>
+      </c>
+      <c r="E86" s="4">
+        <f t="shared" si="0"/>
+        <v>0.64999999999999902</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2514,7 +2522,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>94.496666666666641</v>
+        <v>95.146666666666647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed so Crouton properly animates when displayed after Game is closed.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65.8333333333333</c:v>
+                  <c:v>66.316666666666634</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2393,9 +2393,15 @@
       <c r="C86" s="1">
         <v>0.42638888888888887</v>
       </c>
+      <c r="D86" s="3">
+        <v>10</v>
+      </c>
       <c r="E86" s="4">
         <f t="shared" si="0"/>
-        <v>0.64999999999999902</v>
+        <v>0.48333333333333239</v>
+      </c>
+      <c r="F86" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2522,7 +2528,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>95.146666666666647</v>
+        <v>94.979999999999976</v>
       </c>
     </row>
   </sheetData>
@@ -2567,7 +2573,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.7108187237645071E-2</v>
+        <v>1.7021127254860675E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2576,11 +2582,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>65.8333333333333</v>
+        <v>66.316666666666634</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.69667360400719591</v>
+        <v>0.69821716852670734</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2593,7 +2599,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.20953120039507572</v>
+        <v>0.20846493998736582</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2606,7 +2612,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>7.668700836008327E-2</v>
+        <v>7.6296764231066211E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on moving PlayingCardViews.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,7 +2405,12 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="2"/>
+      <c r="A87" s="2">
+        <v>41928</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0.76527777777777783</v>
+      </c>
       <c r="E87" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
Fixing issues with Fling animation.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66.316666666666634</c:v>
+                  <c:v>71.399999999999963</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2411,16 +2411,39 @@
       <c r="B87" s="1">
         <v>0.76527777777777783</v>
       </c>
-      <c r="E87" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="C87" s="1">
+        <v>0.87847222222222221</v>
+      </c>
+      <c r="D87" s="3">
+        <v>20</v>
+      </c>
+      <c r="E87" s="4">
+        <f t="shared" si="0"/>
+        <v>2.3833333333333315</v>
+      </c>
+      <c r="F87" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
-      <c r="E88" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A88" s="2">
+        <v>41929</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="C88" s="1">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="D88" s="3">
+        <v>30</v>
+      </c>
+      <c r="E88" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6999999999999993</v>
+      </c>
+      <c r="F88" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2533,7 +2556,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>94.979999999999976</v>
+        <v>100.0633333333333</v>
       </c>
     </row>
   </sheetData>
@@ -2578,7 +2601,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.7021127254860675E-2</v>
+        <v>1.6156434258303078E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2587,11 +2610,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>66.316666666666634</v>
+        <v>71.399999999999963</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.69821716852670734</v>
+        <v>0.71354808621206567</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2604,7 +2627,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.20846493998736582</v>
+        <v>0.19787467936973255</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2617,7 +2640,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>7.6296764231066211E-2</v>
+        <v>7.2420800159898754E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issues with CardDisplayLayout onLayout.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71.399999999999963</c:v>
+                  <c:v>73.649999999999963</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+      <selection activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +591,7 @@
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.140625" style="10" bestFit="1" customWidth="1"/>
@@ -2447,10 +2447,24 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
-      <c r="E89" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A89" s="2">
+        <v>41930</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C89" s="1">
+        <v>0.74652777777777779</v>
+      </c>
+      <c r="D89" s="3">
+        <v>20</v>
+      </c>
+      <c r="E89" s="4">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999987</v>
+      </c>
+      <c r="F89" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2556,7 +2570,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>100.0633333333333</v>
+        <v>102.3133333333333</v>
       </c>
     </row>
   </sheetData>
@@ -2601,7 +2615,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.6156434258303078E-2</v>
+        <v>1.580113377207272E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2610,11 +2624,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>71.399999999999963</v>
+        <v>73.649999999999963</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.71354808621206567</v>
+        <v>0.71984752720401379</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2627,7 +2641,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.19787467936973255</v>
+        <v>0.19352316413631335</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2640,7 +2654,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>7.2420800159898754E-2</v>
+        <v>7.0828174887600195E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed scaling problems on Table.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73.649999999999963</c:v>
+                  <c:v>74.349999999999966</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="H88" sqref="H88"/>
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2468,10 +2468,24 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
-      <c r="E90" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A90" s="2">
+        <v>41930</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="C90" s="1">
+        <v>0.79305555555555562</v>
+      </c>
+      <c r="D90" s="3">
+        <v>0</v>
+      </c>
+      <c r="E90" s="4">
+        <f t="shared" si="0"/>
+        <v>0.70000000000000284</v>
+      </c>
+      <c r="F90" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2570,7 +2584,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>102.3133333333333</v>
+        <v>103.01333333333331</v>
       </c>
     </row>
   </sheetData>
@@ -2615,7 +2629,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.580113377207272E-2</v>
+        <v>1.5693761325394774E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2624,11 +2638,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>73.649999999999963</v>
+        <v>74.349999999999966</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.71984752720401379</v>
+        <v>0.72175122961428939</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2641,7 +2655,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.19352316413631335</v>
+        <v>0.19220812839761847</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2654,7 +2668,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>7.0828174887600195E-2</v>
+        <v>7.0346880662697397E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed how card bitmaps are loaded.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.349999999999966</c:v>
+                  <c:v>74.71666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,10 +2489,24 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="2"/>
-      <c r="E91" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A91" s="2">
+        <v>41930</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="C91" s="1">
+        <v>0.81388888888888899</v>
+      </c>
+      <c r="D91" s="3">
+        <v>0</v>
+      </c>
+      <c r="E91" s="4">
+        <f t="shared" si="0"/>
+        <v>0.36666666666666803</v>
+      </c>
+      <c r="F91" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2584,7 +2598,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>103.01333333333331</v>
+        <v>103.37999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2629,7 +2643,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.5693761325394774E-2</v>
+        <v>1.5638098923067004E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2638,11 +2652,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>74.349999999999966</v>
+        <v>74.71666666666664</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.72175122961428939</v>
+        <v>0.72273811826916878</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2655,7 +2669,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.19220812839761847</v>
+        <v>0.19152640742890312</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2668,7 +2682,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>7.0346880662697397E-2</v>
+        <v>7.0097375378861168E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed flip animation to use simple xml animations instead of library. Totes works better.
Closes #5
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.71666666666664</c:v>
+                  <c:v>76.983333333333306</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2510,10 +2510,24 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="2"/>
-      <c r="E92" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A92" s="2">
+        <v>41931</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C92" s="1">
+        <v>0.60833333333333328</v>
+      </c>
+      <c r="D92" s="3">
+        <v>20</v>
+      </c>
+      <c r="E92" s="4">
+        <f t="shared" si="0"/>
+        <v>2.2666666666666653</v>
+      </c>
+      <c r="F92" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2598,7 +2612,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>103.37999999999998</v>
+        <v>105.64666666666665</v>
       </c>
     </row>
   </sheetData>
@@ -2643,7 +2657,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.5638098923067004E-2</v>
+        <v>1.5302580930144508E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2652,11 +2666,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>74.71666666666664</v>
+        <v>76.983333333333306</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.72273811826916878</v>
+        <v>0.72868681769420074</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2669,7 +2683,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.19152640742890312</v>
+        <v>0.1874171767526977</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2682,7 +2696,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>7.0097375378861168E-2</v>
+        <v>6.8593424622957033E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ability to save, load, and delete saved Scratch Pads.
Closes #19
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76.983333333333306</c:v>
+                  <c:v>78.849999999999966</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2531,10 +2531,24 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="2"/>
-      <c r="E93" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A93" s="2">
+        <v>41931</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0.7319444444444444</v>
+      </c>
+      <c r="C93" s="1">
+        <v>0.82361111111111107</v>
+      </c>
+      <c r="D93" s="3">
+        <v>20</v>
+      </c>
+      <c r="E93" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8666666666666669</v>
+      </c>
+      <c r="F93" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2612,7 +2626,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>105.64666666666665</v>
+        <v>107.51333333333331</v>
       </c>
     </row>
   </sheetData>
@@ -2657,7 +2671,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.5302580930144508E-2</v>
+        <v>1.5036894648725742E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2666,11 +2680,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>76.983333333333306</v>
+        <v>78.849999999999966</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.72868681769420074</v>
+        <v>0.73339740807341725</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2683,7 +2697,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.1874171767526977</v>
+        <v>0.18416320456377508</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2696,7 +2710,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>6.8593424622957033E-2</v>
+        <v>6.7402492714081982E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ability to preview scratch pads before loading them.
Closes #20
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.849999999999966</c:v>
+                  <c:v>79.749999999999972</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2552,10 +2552,24 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
-      <c r="E94" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A94" s="2">
+        <v>41932</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0.54583333333333328</v>
+      </c>
+      <c r="C94" s="1">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="D94" s="3">
+        <v>5</v>
+      </c>
+      <c r="E94" s="4">
+        <f t="shared" si="0"/>
+        <v>0.9000000000000018</v>
+      </c>
+      <c r="F94" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2626,7 +2640,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>107.51333333333331</v>
+        <v>108.41333333333331</v>
       </c>
     </row>
   </sheetData>
@@ -2671,7 +2685,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.5036894648725742E-2</v>
+        <v>1.4912064936662158E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2680,11 +2694,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>78.849999999999966</v>
+        <v>79.749999999999972</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.73339740807341725</v>
+        <v>0.73561062599926208</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2697,7 +2711,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.18416320456377508</v>
+        <v>0.18263436231705821</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2710,7 +2724,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>6.7402492714081982E-2</v>
+        <v>6.6842946747017601E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added color picker for scratch pad. Started working on stroke size.
Closes #22
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79.749999999999972</c:v>
+                  <c:v>81.316666666666634</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2573,10 +2573,24 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="2"/>
-      <c r="E95" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A95" s="2">
+        <v>41932</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="C95" s="1">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="D95" s="3">
+        <v>5</v>
+      </c>
+      <c r="E95" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5666666666666689</v>
+      </c>
+      <c r="F95" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2640,7 +2654,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>108.41333333333331</v>
+        <v>109.97999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2685,7 +2699,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.4912064936662158E-2</v>
+        <v>1.4699642359216829E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2694,11 +2708,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>79.749999999999972</v>
+        <v>81.316666666666634</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.73561062599926208</v>
+        <v>0.739376856398133</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2711,7 +2725,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.18263436231705821</v>
+        <v>0.18003273322422261</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2724,7 +2738,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>6.6842946747017601E-2</v>
+        <v>6.5890768018427609E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ability to change stroke size on scratch pad.
Closes #23
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>81.316666666666634</c:v>
+                  <c:v>82.549999999999969</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2594,10 +2594,24 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="2"/>
-      <c r="E96" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A96" s="2">
+        <v>41933</v>
+      </c>
+      <c r="B96" s="1">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="C96" s="1">
+        <v>0.56527777777777777</v>
+      </c>
+      <c r="D96" s="3">
+        <v>5</v>
+      </c>
+      <c r="E96" s="4">
+        <f t="shared" si="0"/>
+        <v>1.2333333333333341</v>
+      </c>
+      <c r="F96" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2654,7 +2668,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>109.97999999999998</v>
+        <v>111.21333333333331</v>
       </c>
     </row>
   </sheetData>
@@ -2699,7 +2713,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.4699642359216829E-2</v>
+        <v>1.4536626303800504E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2708,11 +2722,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>81.316666666666634</v>
+        <v>82.549999999999969</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.739376856398133</v>
+        <v>0.74226711425488545</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2725,7 +2739,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.18003273322422261</v>
+        <v>0.17803620668984538</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2738,7 +2752,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>6.5890768018427609E-2</v>
+        <v>6.5160052751468661E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed dealer aspect from game.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.549999999999969</c:v>
+                  <c:v>83.44999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,61 +2614,75 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="2"/>
-      <c r="E97" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>41933</v>
+      </c>
+      <c r="B97" s="1">
+        <v>0.72569444444444453</v>
+      </c>
+      <c r="C97" s="1">
+        <v>0.76666666666666661</v>
+      </c>
+      <c r="D97" s="3">
+        <v>5</v>
+      </c>
+      <c r="E97" s="4">
+        <f t="shared" si="0"/>
+        <v>0.89999999999999647</v>
+      </c>
+      <c r="F97" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="E98" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="E99" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="E100" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="E101" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="E102" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E103" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>9</v>
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>111.21333333333331</v>
+        <v>112.1133333333333</v>
       </c>
     </row>
   </sheetData>
@@ -2713,7 +2727,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.4536626303800504E-2</v>
+        <v>1.4419932211452699E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2722,11 +2736,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>82.549999999999969</v>
+        <v>83.44999999999996</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.74226711425488545</v>
+        <v>0.74433608848189325</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2739,7 +2753,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.17803620668984538</v>
+        <v>0.17660700481655472</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2752,7 +2766,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>6.5160052751468661E-2</v>
+        <v>6.4636974490099322E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed card layout feature not working properly. Added card layout icon to actionbar.
Closes #27
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>83.44999999999996</c:v>
+                  <c:v>84.783333333333289</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2636,10 +2636,24 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="2"/>
-      <c r="E98" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A98" s="2">
+        <v>41935</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0.93680555555555556</v>
+      </c>
+      <c r="C98" s="1">
+        <v>0.99583333333333324</v>
+      </c>
+      <c r="D98" s="3">
+        <v>5</v>
+      </c>
+      <c r="E98" s="4">
+        <f t="shared" si="0"/>
+        <v>1.333333333333331</v>
+      </c>
+      <c r="F98" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2682,7 +2696,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>112.1133333333333</v>
+        <v>113.44666666666663</v>
       </c>
     </row>
   </sheetData>
@@ -2727,7 +2741,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.4419932211452699E-2</v>
+        <v>1.4250455426926018E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2736,11 +2750,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>83.44999999999996</v>
+        <v>84.783333333333289</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.74433608848189325</v>
+        <v>0.74734089439971785</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2753,7 +2767,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.17660700481655472</v>
+        <v>0.17453135100193928</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2766,7 +2780,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>6.4636974490099322E-2</v>
+        <v>6.3877299171416838E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ability to send card straight to table when table is open and straight from table.
Closes #28
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>84.783333333333289</c:v>
+                  <c:v>85.783333333333289</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,10 +2657,24 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="2"/>
-      <c r="E99" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A99" s="2">
+        <v>41936</v>
+      </c>
+      <c r="B99" s="1">
+        <v>0</v>
+      </c>
+      <c r="C99" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D99" s="3">
+        <v>0</v>
+      </c>
+      <c r="E99" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F99" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2696,7 +2710,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>113.44666666666663</v>
+        <v>114.44666666666663</v>
       </c>
     </row>
   </sheetData>
@@ -2741,7 +2755,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.4250455426926018E-2</v>
+        <v>1.4125939302149476E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2750,11 +2764,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>84.783333333333289</v>
+        <v>85.783333333333289</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.74734089439971785</v>
+        <v>0.74954855245529206</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2767,7 +2781,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.17453135100193928</v>
+        <v>0.17300634939127402</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2780,7 +2794,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>6.3877299171416838E-2</v>
+        <v>6.331915885128446E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed unneeded drawables. Switched to other Iconify icons. Fixed issue with DeviceListActivity.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85.783333333333289</c:v>
+                  <c:v>86.19999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2678,10 +2678,24 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="2"/>
-      <c r="E100" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A100" s="2">
+        <v>41939</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C100" s="1">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="D100" s="3">
+        <v>0</v>
+      </c>
+      <c r="E100" s="4">
+        <f t="shared" si="0"/>
+        <v>0.41666666666666519</v>
+      </c>
+      <c r="F100" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2710,7 +2724,7 @@
       </c>
       <c r="E104" s="4">
         <f>SUM(E2:E103)</f>
-        <v>114.44666666666663</v>
+        <v>114.8633333333333</v>
       </c>
     </row>
   </sheetData>
@@ -2755,7 +2769,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.4125939302149476E-2</v>
+        <v>1.4074697466554459E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2764,11 +2778,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>85.783333333333289</v>
+        <v>86.19999999999996</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.74954855245529206</v>
+        <v>0.75045706491772823</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2781,7 +2795,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.17300634939127402</v>
+        <v>0.17237876897182164</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2794,7 +2808,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>6.331915885128446E-2</v>
+        <v>6.3089468643895655E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued working on draw and discard piles on table. And other small changes.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>86.19999999999996</c:v>
+                  <c:v>89.033333333333303</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -579,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E103" si="0">IF(AND(NOT(ISBLANK(B4)),NOT(ISBLANK(C4))), (C4-B4) * 24 - D4/60, "")</f>
+        <f t="shared" ref="E4:E121" si="0">IF(AND(NOT(ISBLANK(B4)),NOT(ISBLANK(C4))), (C4-B4) * 24 - D4/60, "")</f>
         <v>0.33333333333333748</v>
       </c>
       <c r="F4" t="s">
@@ -2699,32 +2699,114 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="2"/>
-      <c r="E101" s="4" t="str">
+      <c r="A101" s="2">
+        <v>41939</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0.92222222222222217</v>
+      </c>
+      <c r="C101" s="1">
+        <v>0.99236111111111114</v>
+      </c>
+      <c r="D101" s="3">
+        <v>0</v>
+      </c>
+      <c r="E101" s="4">
+        <f t="shared" si="0"/>
+        <v>1.6833333333333353</v>
+      </c>
+      <c r="F101" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>41940</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0.52847222222222223</v>
+      </c>
+      <c r="C102" s="1">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="D102" s="3">
+        <v>0</v>
+      </c>
+      <c r="E102" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1500000000000012</v>
+      </c>
+      <c r="F102" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="2"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="2"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="2"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="2"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="2"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="2"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="2"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="2"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="2"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="2"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="2"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="2"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E121" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="2"/>
-      <c r="E102" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E103" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>9</v>
       </c>
-      <c r="E104" s="4">
-        <f>SUM(E2:E103)</f>
-        <v>114.8633333333333</v>
+      <c r="E122" s="4">
+        <f>SUM(E2:E121)</f>
+        <v>117.69666666666664</v>
       </c>
     </row>
   </sheetData>
@@ -2764,12 +2846,12 @@
         <v>6</v>
       </c>
       <c r="B2" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$103,A2,Sheet1!$E$2:$E$103)</f>
+        <f>SUMIF(Sheet1!$F$2:$F$121,A2,Sheet1!$E$2:$E$121)</f>
         <v>1.6166666666666663</v>
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.4074697466554459E-2</v>
+        <v>1.3735874706165567E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2777,12 +2859,12 @@
         <v>7</v>
       </c>
       <c r="B3" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$103,A3,Sheet1!$E$2:$E$103)</f>
-        <v>86.19999999999996</v>
+        <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
+        <v>89.033333333333303</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.75045706491772823</v>
+        <v>0.75646435752924179</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2790,12 +2872,12 @@
         <v>8</v>
       </c>
       <c r="B4" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$103,A4,Sheet1!$E$2:$E$103)</f>
+        <f>SUMIF(Sheet1!$F$2:$F$121,A4,Sheet1!$E$2:$E$121)</f>
         <v>19.799999999999997</v>
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.17237876897182164</v>
+        <v>0.1682290634115948</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2803,12 +2885,12 @@
         <v>12</v>
       </c>
       <c r="B5" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$103,A5,Sheet1!$E$2:$E$103)</f>
+        <f>SUMIF(Sheet1!$F$2:$F$121,A5,Sheet1!$E$2:$E$121)</f>
         <v>7.2466666666666653</v>
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>6.3089468643895655E-2</v>
+        <v>6.1570704352997829E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ability to set sides of screen as player.
Closes #34
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89.033333333333303</c:v>
+                  <c:v>90.649999999999963</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,7 +2741,25 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="2"/>
+      <c r="A103" s="2">
+        <v>41942</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="C103" s="1">
+        <v>0.87986111111111109</v>
+      </c>
+      <c r="D103" s="3">
+        <v>0</v>
+      </c>
+      <c r="E103" s="4">
+        <f t="shared" si="0"/>
+        <v>1.6166666666666663</v>
+      </c>
+      <c r="F103" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
@@ -2806,7 +2824,7 @@
       </c>
       <c r="E122" s="4">
         <f>SUM(E2:E121)</f>
-        <v>117.69666666666664</v>
+        <v>119.3133333333333</v>
       </c>
     </row>
   </sheetData>
@@ -2851,7 +2869,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.3735874706165567E-2</v>
+        <v>1.3549756942504331E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2860,11 +2878,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>89.033333333333303</v>
+        <v>90.649999999999963</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.75646435752924179</v>
+        <v>0.75976420629155716</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2877,7 +2895,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.1682290634115948</v>
+        <v>0.16594960049170257</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2890,7 +2908,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>6.1570704352997829E-2</v>
+        <v>6.0736436274235917E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on fixing issues with SlidingFrameLayout.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93.416666666666629</c:v>
+                  <c:v>95.283333333333289</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2783,7 +2783,25 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="2"/>
+      <c r="A105" s="2">
+        <v>41945</v>
+      </c>
+      <c r="B105" s="1">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="C105" s="1">
+        <v>0.1013888888888889</v>
+      </c>
+      <c r="D105" s="3">
+        <v>20</v>
+      </c>
+      <c r="E105" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8666666666666669</v>
+      </c>
+      <c r="F105" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
@@ -2842,7 +2860,7 @@
       </c>
       <c r="E122" s="4">
         <f>SUM(E2:E121)</f>
-        <v>122.07999999999997</v>
+        <v>123.94666666666663</v>
       </c>
     </row>
   </sheetData>
@@ -2887,7 +2905,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.3242682394058541E-2</v>
+        <v>1.3043244406196216E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2896,11 +2914,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>93.416666666666629</v>
+        <v>95.283333333333289</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.7652086063783311</v>
+        <v>0.76874462134251287</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2913,7 +2931,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.16218872870249021</v>
+        <v>0.15974612736660934</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2926,7 +2944,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>5.9359982525120147E-2</v>
+        <v>5.8466006884681593E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issue with cards being dragged after a card was sent to the table or when sent to the player.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95.283333333333289</c:v>
+                  <c:v>97.216666666666626</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2804,7 +2804,25 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="2"/>
+      <c r="A106" s="2">
+        <v>41949</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0.83611111111111114</v>
+      </c>
+      <c r="C106" s="1">
+        <v>0.92013888888888884</v>
+      </c>
+      <c r="D106" s="3">
+        <v>5</v>
+      </c>
+      <c r="E106" s="4">
+        <f t="shared" si="0"/>
+        <v>1.9333333333333316</v>
+      </c>
+      <c r="F106" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
@@ -2860,7 +2878,7 @@
       </c>
       <c r="E122" s="4">
         <f>SUM(E2:E121)</f>
-        <v>123.94666666666663</v>
+        <v>125.87999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2905,7 +2923,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.3043244406196216E-2</v>
+        <v>1.2842919182290012E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2914,11 +2932,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>95.283333333333289</v>
+        <v>97.216666666666626</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.76874462134251287</v>
+        <v>0.77229636691028491</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2931,7 +2949,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.15974612736660934</v>
+        <v>0.15729265967588182</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2944,7 +2962,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>5.8466006884681593E-2</v>
+        <v>5.7568054231543278E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added draw piles and discard piles to table.
Closes #29
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -59,15 +59,19 @@
   <si>
     <t>Percentage</t>
   </si>
+  <si>
+    <t>Total:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="0&quot; mins&quot;"/>
     <numFmt numFmtId="166" formatCode="0.0#&quot; hours&quot;"/>
+    <numFmt numFmtId="169" formatCode="#&quot; days&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -114,7 +118,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -129,6 +133,7 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,6 +164,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -219,7 +225,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>97.216666666666626</c:v>
+                  <c:v>101.29999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -579,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J122"/>
+  <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2825,46 +2831,130 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="2"/>
+      <c r="A107" s="2">
+        <v>41950</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0.7270833333333333</v>
+      </c>
+      <c r="C107" s="1">
+        <v>0.87222222222222223</v>
+      </c>
+      <c r="D107" s="3">
+        <v>30</v>
+      </c>
+      <c r="E107" s="4">
+        <f t="shared" si="0"/>
+        <v>2.9833333333333343</v>
+      </c>
+      <c r="F107" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="2"/>
+      <c r="A108" s="2">
+        <v>41951</v>
+      </c>
+      <c r="B108" s="1">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C108" s="1">
+        <v>0.65347222222222223</v>
+      </c>
+      <c r="D108" s="3">
+        <v>15</v>
+      </c>
+      <c r="E108" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000005</v>
+      </c>
+      <c r="F108" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
+      <c r="E109" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
+      <c r="E110" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
+      <c r="E111" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
+      <c r="E112" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
+      <c r="E113" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
+      <c r="E114" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
+      <c r="E115" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
+      <c r="E116" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
+      <c r="E117" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
+      <c r="E118" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
+      <c r="E119" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
+      <c r="E120" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E121" s="4" t="str">
@@ -2878,8 +2968,11 @@
       </c>
       <c r="E122" s="4">
         <f>SUM(E2:E121)</f>
-        <v>125.87999999999997</v>
-      </c>
+        <v>129.96333333333328</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E123" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2889,16 +2982,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C9" activeCellId="1" sqref="A7 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2923,7 +3016,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.2842919182290012E-2</v>
+        <v>1.2439405986303831E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2932,11 +3025,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>97.216666666666626</v>
+        <v>101.29999999999995</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.77229636691028491</v>
+        <v>0.7794506142758213</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2949,7 +3042,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.15729265967588182</v>
+        <v>0.15235066300751499</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2962,7 +3055,16 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>5.7568054231543278E-2</v>
+        <v>5.5759316730359859E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="10">
+        <f>SUM(B2:B5)</f>
+        <v>129.96333333333328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added multi-touch support to CardDisplayLayout.
Closes #41
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -71,7 +71,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="0&quot; mins&quot;"/>
     <numFmt numFmtId="166" formatCode="0.0#&quot; hours&quot;"/>
-    <numFmt numFmtId="169" formatCode="#&quot; days&quot;"/>
+    <numFmt numFmtId="167" formatCode="#&quot; days&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -133,7 +133,7 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,7 +164,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -225,7 +224,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>101.29999999999995</c:v>
+                  <c:v>102.79999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -587,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2856,27 +2855,41 @@
         <v>41951</v>
       </c>
       <c r="B108" s="1">
-        <v>0.59722222222222221</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="C108" s="1">
-        <v>0.65347222222222223</v>
+        <v>0.15347222222222223</v>
       </c>
       <c r="D108" s="3">
         <v>15</v>
       </c>
       <c r="E108" s="4">
         <f t="shared" si="0"/>
-        <v>1.1000000000000005</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F108" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="2"/>
-      <c r="E109" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A109" s="2">
+        <v>41951</v>
+      </c>
+      <c r="B109" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C109" s="1">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="D109" s="3">
+        <v>10</v>
+      </c>
+      <c r="E109" s="4">
+        <f t="shared" si="0"/>
+        <v>1.500000000000002</v>
+      </c>
+      <c r="F109" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -2968,7 +2981,7 @@
       </c>
       <c r="E122" s="4">
         <f>SUM(E2:E121)</f>
-        <v>129.96333333333328</v>
+        <v>131.46333333333328</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3016,7 +3029,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.2439405986303831E-2</v>
+        <v>1.2297472045437258E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3025,11 +3038,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>101.29999999999995</v>
+        <v>102.79999999999995</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.7794506142758213</v>
+        <v>0.78196708841502061</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3042,7 +3055,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.15235066300751499</v>
+        <v>0.15061233804102542</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3055,7 +3068,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>5.5759316730359859E-2</v>
+        <v>5.5123101498516708E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3064,7 +3077,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUM(B2:B5)</f>
-        <v>129.96333333333328</v>
+        <v>131.46333333333328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added undo/redo functionality to ScratchPadView.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -224,7 +224,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>102.79999999999995</c:v>
+                  <c:v>105.48333333333329</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -587,7 +587,7 @@
   <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2893,10 +2893,24 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="2"/>
-      <c r="E110" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A110" s="2">
+        <v>41951</v>
+      </c>
+      <c r="B110" s="1">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="C110" s="1">
+        <v>0.84166666666666667</v>
+      </c>
+      <c r="D110" s="3">
+        <v>25</v>
+      </c>
+      <c r="E110" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6833333333333331</v>
+      </c>
+      <c r="F110" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -2981,7 +2995,7 @@
       </c>
       <c r="E122" s="4">
         <f>SUM(E2:E121)</f>
-        <v>131.46333333333328</v>
+        <v>134.14666666666662</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3029,7 +3043,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.2297472045437258E-2</v>
+        <v>1.2051485935791672E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3038,11 +3052,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>102.79999999999995</v>
+        <v>105.48333333333329</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.78196708841502061</v>
+        <v>0.78632839677964417</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3055,7 +3069,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.15061233804102542</v>
+        <v>0.14759964218268565</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3068,7 +3082,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>5.5123101498516708E-2</v>
+        <v>5.4020475101878553E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3077,7 +3091,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUM(B2:B5)</f>
-        <v>131.46333333333328</v>
+        <v>134.14666666666662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many small changes to menu population and items.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -224,7 +224,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105.48333333333329</c:v>
+                  <c:v>107.8833333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -587,7 +587,7 @@
   <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,10 +2914,24 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="2"/>
-      <c r="E111" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A111" s="2">
+        <v>41952</v>
+      </c>
+      <c r="B111" s="1">
+        <v>0.52638888888888891</v>
+      </c>
+      <c r="C111" s="1">
+        <v>0.63680555555555551</v>
+      </c>
+      <c r="D111" s="3">
+        <v>15</v>
+      </c>
+      <c r="E111" s="4">
+        <f t="shared" si="0"/>
+        <v>2.3999999999999986</v>
+      </c>
+      <c r="F111" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -2995,7 +3009,7 @@
       </c>
       <c r="E122" s="4">
         <f>SUM(E2:E121)</f>
-        <v>134.14666666666662</v>
+        <v>136.54666666666662</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3043,7 +3057,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.2051485935791672E-2</v>
+        <v>1.1839664095303194E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3052,11 +3066,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>105.48333333333329</v>
+        <v>107.8833333333333</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.78632839677964417</v>
+        <v>0.79008397617420167</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3069,7 +3083,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.14759964218268565</v>
+        <v>0.14500537056928037</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3082,7 +3096,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>5.4020475101878553E-2</v>
+        <v>5.3070989161214728E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3091,7 +3105,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUM(B2:B5)</f>
-        <v>134.14666666666662</v>
+        <v>136.54666666666662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added long-press edge swipe to assign players to sides.
Closes #45
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -224,7 +224,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>107.8833333333333</c:v>
+                  <c:v>109.74999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -587,7 +587,7 @@
   <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,10 +2935,24 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="2"/>
-      <c r="E112" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A112" s="2">
+        <v>41953</v>
+      </c>
+      <c r="B112" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="C112" s="1">
+        <v>0.61944444444444446</v>
+      </c>
+      <c r="D112" s="3">
+        <v>15</v>
+      </c>
+      <c r="E112" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8666666666666671</v>
+      </c>
+      <c r="F112" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3009,7 +3023,7 @@
       </c>
       <c r="E122" s="4">
         <f>SUM(E2:E121)</f>
-        <v>136.54666666666662</v>
+        <v>138.4133333333333</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3057,7 +3071,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.1839664095303194E-2</v>
+        <v>1.1679992293613332E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3066,11 +3080,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>107.8833333333333</v>
+        <v>109.74999999999997</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.79008397617420167</v>
+        <v>0.79291494075715252</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3083,7 +3097,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.14500537056928037</v>
+        <v>0.14304980252384164</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3096,7 +3110,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>5.3070989161214728E-2</v>
+        <v>5.2355264425392546E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3105,7 +3119,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUM(B2:B5)</f>
-        <v>136.54666666666662</v>
+        <v>138.4133333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ListView scrolls to currently used background.
Closes #48
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -224,7 +224,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>109.74999999999997</c:v>
+                  <c:v>110.18333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -587,7 +587,7 @@
   <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2955,78 +2955,92 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="2"/>
-      <c r="E113" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>41956</v>
+      </c>
+      <c r="B113" s="1">
+        <v>0.64374999999999993</v>
+      </c>
+      <c r="C113" s="1">
+        <v>0.66527777777777775</v>
+      </c>
+      <c r="D113" s="3">
+        <v>5</v>
+      </c>
+      <c r="E113" s="4">
+        <f t="shared" si="0"/>
+        <v>0.43333333333333418</v>
+      </c>
+      <c r="F113" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="E114" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="E115" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="E116" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="E117" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="E118" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="E119" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="E120" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E121" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>9</v>
       </c>
       <c r="E122" s="4">
         <f>SUM(E2:E121)</f>
-        <v>138.4133333333333</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>138.84666666666664</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E123" s="14"/>
     </row>
   </sheetData>
@@ -3071,7 +3085,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.1679992293613332E-2</v>
+        <v>1.1643539636049359E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3080,11 +3094,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>109.74999999999997</v>
+        <v>110.18333333333331</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.79291494075715252</v>
+        <v>0.79356124261775585</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3097,7 +3111,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.14304980252384164</v>
+        <v>0.14260335141883135</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3110,7 +3124,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>5.2355264425392546E-2</v>
+        <v>5.2191866327363522E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3119,7 +3133,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUM(B2:B5)</f>
-        <v>138.4133333333333</v>
+        <v>138.84666666666664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added outlines to discard/draw card piles. Improved CardHolder selection lists. Other small fixes.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -224,7 +224,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110.18333333333331</c:v>
+                  <c:v>116.13333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2977,24 +2977,66 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="2"/>
-      <c r="E114" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A114" s="2">
+        <v>41956</v>
+      </c>
+      <c r="B114" s="1">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="C114" s="1">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="D114" s="3">
+        <v>15</v>
+      </c>
+      <c r="E114" s="4">
+        <f t="shared" si="0"/>
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="F114" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="2"/>
-      <c r="E115" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A115" s="2">
+        <v>41957</v>
+      </c>
+      <c r="B115" s="1">
+        <v>0.78125</v>
+      </c>
+      <c r="C115" s="1">
+        <v>0.91527777777777775</v>
+      </c>
+      <c r="D115" s="3">
+        <v>45</v>
+      </c>
+      <c r="E115" s="4">
+        <f t="shared" si="0"/>
+        <v>2.4666666666666659</v>
+      </c>
+      <c r="F115" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="2"/>
-      <c r="E116" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A116" s="2">
+        <v>41958</v>
+      </c>
+      <c r="B116" s="1">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C116" s="1">
+        <v>0.7319444444444444</v>
+      </c>
+      <c r="D116" s="3">
+        <v>20</v>
+      </c>
+      <c r="E116" s="4">
+        <f t="shared" si="0"/>
+        <v>2.899999999999999</v>
+      </c>
+      <c r="F116" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3037,7 +3079,7 @@
       </c>
       <c r="E122" s="4">
         <f>SUM(E2:E121)</f>
-        <v>138.84666666666664</v>
+        <v>144.79666666666665</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3085,7 +3127,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.1643539636049359E-2</v>
+        <v>1.1165082069108405E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3094,11 +3136,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>110.18333333333331</v>
+        <v>116.13333333333331</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.79356124261775585</v>
+        <v>0.80204424595409662</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3111,7 +3153,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.14260335141883135</v>
+        <v>0.13674347936186379</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3124,7 +3166,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>5.2191866327363522E-2</v>
+        <v>5.0047192614931291E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3133,7 +3175,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUM(B2:B5)</f>
-        <v>138.84666666666664</v>
+        <v>144.79666666666662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed GameMessage handling to use Queue.
Closes #54
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -224,7 +224,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>116.13333333333331</c:v>
+                  <c:v>117.26666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -587,7 +587,7 @@
   <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3040,10 +3040,24 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="2"/>
-      <c r="E117" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A117" s="2">
+        <v>41959</v>
+      </c>
+      <c r="B117" s="1">
+        <v>0.97986111111111107</v>
+      </c>
+      <c r="C117" s="1">
+        <v>1.0305555555555554</v>
+      </c>
+      <c r="D117" s="3">
+        <v>5</v>
+      </c>
+      <c r="E117" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1333333333333317</v>
+      </c>
+      <c r="F117" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3079,7 +3093,7 @@
       </c>
       <c r="E122" s="4">
         <f>SUM(E2:E121)</f>
-        <v>144.79666666666665</v>
+        <v>145.92999999999998</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3127,7 +3141,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.1165082069108405E-2</v>
+        <v>1.1078370908426416E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3136,11 +3150,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>116.13333333333331</v>
+        <v>117.26666666666664</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.80204424595409662</v>
+        <v>0.80358162589369342</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3153,7 +3167,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.13674347936186379</v>
+        <v>0.13568149112588229</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3166,7 +3180,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>5.0047192614931291E-2</v>
+        <v>4.9658512071998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3175,7 +3189,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUM(B2:B5)</f>
-        <v>144.79666666666662</v>
+        <v>145.92999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issue with trying to connect with older or newer versions of Deck.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -224,7 +224,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>117.5333333333333</c:v>
+                  <c:v>117.84999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -587,7 +587,7 @@
   <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3082,10 +3082,24 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="2"/>
-      <c r="E119" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A119" s="2">
+        <v>41960</v>
+      </c>
+      <c r="B119" s="1">
+        <v>0.54722222222222217</v>
+      </c>
+      <c r="C119" s="1">
+        <v>0.56388888888888888</v>
+      </c>
+      <c r="D119" s="3">
+        <v>5</v>
+      </c>
+      <c r="E119" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31666666666666793</v>
+      </c>
+      <c r="F119" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3107,7 +3121,7 @@
       </c>
       <c r="E122" s="4">
         <f>SUM(E2:E121)</f>
-        <v>146.19666666666663</v>
+        <v>146.51333333333329</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3155,7 +3169,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.1058163660822179E-2</v>
+        <v>1.1034263093233836E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3164,11 +3178,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>117.5333333333333</v>
+        <v>117.84999999999997</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.80393989831049495</v>
+        <v>0.80436365290986034</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3181,7 +3195,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.13543400442326547</v>
+        <v>0.13514128406970927</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3194,7 +3208,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>4.9567933605417364E-2</v>
+        <v>4.9460799927196618E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3203,7 +3217,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUM(B2:B5)</f>
-        <v>146.19666666666663</v>
+        <v>146.51333333333329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed GameSaves over to use CardViews. Removed 'com.daimajia.swipelayout:library:1.1.7@aar' from build.gradle.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="13110"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -224,7 +224,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>118.49999999999997</c:v>
+                  <c:v>120.66666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -584,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J123"/>
+  <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E121" si="0">IF(AND(NOT(ISBLANK(B4)),NOT(ISBLANK(C4))), (C4-B4) * 24 - D4/60, "")</f>
+        <f t="shared" ref="E4:E151" si="0">IF(AND(NOT(ISBLANK(B4)),NOT(ISBLANK(C4))), (C4-B4) * 24 - D4/60, "")</f>
         <v>0.33333333333333748</v>
       </c>
       <c r="F4" t="s">
@@ -3124,22 +3124,130 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E121" s="4" t="str">
+      <c r="A121" s="2">
+        <v>41968</v>
+      </c>
+      <c r="B121" s="1">
+        <v>0.59791666666666665</v>
+      </c>
+      <c r="C121" s="1">
+        <v>0.68819444444444444</v>
+      </c>
+      <c r="D121" s="3">
+        <v>0</v>
+      </c>
+      <c r="E121" s="4">
+        <f t="shared" si="0"/>
+        <v>2.166666666666667</v>
+      </c>
+      <c r="F121" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="2"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="2"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="2"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="2"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="2"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="2"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="2"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="2"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="2"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="2"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="2"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="2"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="2"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E151" s="4" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>9</v>
       </c>
-      <c r="E122" s="4">
-        <f>SUM(E2:E121)</f>
-        <v>147.1633333333333</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E123" s="14"/>
+      <c r="E152" s="4">
+        <f>SUM(E2:E151)</f>
+        <v>149.32999999999996</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E153" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3178,12 +3286,12 @@
         <v>6</v>
       </c>
       <c r="B2" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$121,A2,Sheet1!$E$2:$E$121)</f>
+        <f>SUMIF(Sheet1!$F$2:$F$151,A2,Sheet1!$E$2:$E$151)</f>
         <v>1.6166666666666663</v>
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.0985526285986093E-2</v>
+        <v>1.0826134511931068E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3191,12 +3299,12 @@
         <v>7</v>
       </c>
       <c r="B3" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$121,A3,Sheet1!$E$2:$E$121)</f>
-        <v>118.49999999999997</v>
+        <f>SUMIF(Sheet1!$F$2:$F$151,A3,Sheet1!$E$2:$E$151)</f>
+        <v>120.66666666666664</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.80522775147794967</v>
+        <v>0.80805375119980349</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3204,12 +3312,12 @@
         <v>8</v>
       </c>
       <c r="B4" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$121,A4,Sheet1!$E$2:$E$121)</f>
+        <f>SUMIF(Sheet1!$F$2:$F$151,A4,Sheet1!$E$2:$E$151)</f>
         <v>19.799999999999997</v>
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.13454438379125236</v>
+        <v>0.13259224536261971</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3217,12 +3325,12 @@
         <v>12</v>
       </c>
       <c r="B5" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$121,A5,Sheet1!$E$2:$E$121)</f>
+        <f>SUMIF(Sheet1!$F$2:$F$151,A5,Sheet1!$E$2:$E$151)</f>
         <v>7.2466666666666653</v>
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>4.9242338444811892E-2</v>
+        <v>4.8527868925645659E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3231,7 +3339,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUM(B2:B5)</f>
-        <v>147.1633333333333</v>
+        <v>149.32999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed over to different Icon provider. Added 'Libraries Used' to InfoActivity. Enabled Up navigation for Activities. Added ad to InfoActivity. Began adding 'Acknowledgments' to InfoActivity. Started publishing to Google Play Store.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -224,7 +224,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120.66666666666664</c:v>
+                  <c:v>124.38333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -587,7 +587,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122"/>
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3145,10 +3145,46 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="2"/>
+      <c r="A122" s="2">
+        <v>41974</v>
+      </c>
+      <c r="B122" s="1">
+        <v>0.80625000000000002</v>
+      </c>
+      <c r="C122" s="1">
+        <v>0.85486111111111107</v>
+      </c>
+      <c r="D122" s="3">
+        <v>5</v>
+      </c>
+      <c r="E122" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0833333333333319</v>
+      </c>
+      <c r="F122" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="2"/>
+      <c r="A123" s="2">
+        <v>41974</v>
+      </c>
+      <c r="B123" s="1">
+        <v>0.90208333333333324</v>
+      </c>
+      <c r="C123" s="1">
+        <v>1.0152777777777777</v>
+      </c>
+      <c r="D123" s="3">
+        <v>5</v>
+      </c>
+      <c r="E123" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6333333333333342</v>
+      </c>
+      <c r="F123" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
@@ -3243,7 +3279,7 @@
       </c>
       <c r="E152" s="4">
         <f>SUM(E2:E151)</f>
-        <v>149.32999999999996</v>
+        <v>153.04666666666662</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -3291,7 +3327,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.0826134511931068E-2</v>
+        <v>1.0563226902469835E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3300,11 +3336,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$151,A3,Sheet1!$E$2:$E$151)</f>
-        <v>120.66666666666664</v>
+        <v>124.38333333333331</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.80805375119980349</v>
+        <v>0.81271507601167403</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3317,7 +3353,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.13259224536261971</v>
+        <v>0.12937230474365119</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3330,7 +3366,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>4.8527868925645659E-2</v>
+        <v>4.7349392342204998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3339,7 +3375,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUM(B2:B5)</f>
-        <v>149.32999999999998</v>
+        <v>153.04666666666662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issue with info button in MainActivity.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -224,7 +224,7 @@
                   <c:v>1.6166666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>124.38333333333331</c:v>
+                  <c:v>124.66666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19.799999999999997</c:v>
@@ -587,7 +587,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D124" sqref="D124"/>
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3173,14 +3173,14 @@
         <v>0.90208333333333324</v>
       </c>
       <c r="C123" s="1">
-        <v>1.0152777777777777</v>
+        <v>1.0270833333333333</v>
       </c>
       <c r="D123" s="3">
         <v>5</v>
       </c>
       <c r="E123" s="4">
         <f t="shared" si="0"/>
-        <v>2.6333333333333342</v>
+        <v>2.9166666666666692</v>
       </c>
       <c r="F123" t="s">
         <v>7</v>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="E152" s="4">
         <f>SUM(E2:E151)</f>
-        <v>153.04666666666662</v>
+        <v>153.32999999999996</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -3327,7 +3327,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.0563226902469835E-2</v>
+        <v>1.0543707471901561E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3336,11 +3336,11 @@
       </c>
       <c r="B3" s="10">
         <f>SUMIF(Sheet1!$F$2:$F$151,A3,Sheet1!$E$2:$E$151)</f>
-        <v>124.38333333333331</v>
+        <v>124.66666666666664</v>
       </c>
       <c r="C3" s="12">
         <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.81271507601167403</v>
+        <v>0.81306115350333696</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3353,7 +3353,7 @@
       </c>
       <c r="C4" s="12">
         <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.12937230474365119</v>
+        <v>0.12913324202700058</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3366,7 +3366,7 @@
       </c>
       <c r="C5" s="12">
         <f>B5/SUM($B$2:$B$5)</f>
-        <v>4.7349392342204998E-2</v>
+        <v>4.7261896997760816E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3375,7 +3375,7 @@
       </c>
       <c r="B6" s="10">
         <f>SUM(B2:B5)</f>
-        <v>153.04666666666662</v>
+        <v>153.32999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished initial revision of GameCreatorWizardActivity.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Delta</t>
   </si>
   <si>
-    <t>Activity</t>
-  </si>
-  <si>
     <t>Documentation</t>
   </si>
   <si>
@@ -48,19 +45,13 @@
     <t>Total Time:</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Hours</t>
-  </si>
-  <si>
     <t>Planning</t>
   </si>
   <si>
-    <t>Percentage</t>
+    <t>Game Creator Wizard</t>
   </si>
   <si>
-    <t>Total:</t>
+    <t>Task</t>
   </si>
 </sst>
 </file>
@@ -118,7 +109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -128,9 +119,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -147,154 +136,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Hours</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="1"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Documentation</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Coding</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Testing</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Planning</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.6166666666666663</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>124.66666666666664</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.2466666666666653</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="1"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>185738</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,7 +428,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+      <selection activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,10 +438,10 @@
     <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -620,7 +461,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -641,7 +482,7 @@
         <v>0.88333333333333286</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -662,7 +503,7 @@
         <v>0.73333333333333339</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -683,7 +524,7 @@
         <v>0.33333333333333748</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -704,7 +545,7 @@
         <v>0.93333333333333268</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -725,7 +566,7 @@
         <v>1.0666666666666682</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -746,7 +587,7 @@
         <v>0.53333333333333677</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -767,7 +608,7 @@
         <v>0.91666666666666552</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -788,7 +629,7 @@
         <v>0.63333333333333075</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -809,7 +650,7 @@
         <v>1.5999999999999988</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -830,7 +671,7 @@
         <v>1.45</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -851,7 +692,7 @@
         <v>1.3999999999999995</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -872,7 +713,7 @@
         <v>1.1333333333333346</v>
       </c>
       <c r="F13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -893,7 +734,7 @@
         <v>0.56666666666666465</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -914,7 +755,7 @@
         <v>0.36666666666666775</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -935,7 +776,7 @@
         <v>0.63333333333333075</v>
       </c>
       <c r="F16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -956,7 +797,7 @@
         <v>1.2999999999999998</v>
       </c>
       <c r="F17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -977,7 +818,7 @@
         <v>1.6833333333333347</v>
       </c>
       <c r="F18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -998,7 +839,7 @@
         <v>0.6166666666666667</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1019,7 +860,7 @@
         <v>0.8166666666666661</v>
       </c>
       <c r="F20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1040,7 +881,7 @@
         <v>0.26666666666666544</v>
       </c>
       <c r="F21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1062,7 +903,7 @@
         <v>0.53333333333333099</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1083,7 +924,7 @@
         <v>0.5333333333333341</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1104,7 +945,7 @@
         <v>1.3500000000000023</v>
       </c>
       <c r="F24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1125,7 +966,7 @@
         <v>0.76666666666666816</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1146,7 +987,7 @@
         <v>0.36666666666666536</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1167,7 +1008,7 @@
         <v>1.3</v>
       </c>
       <c r="F27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1188,7 +1029,7 @@
         <v>2.833333333333333</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1209,7 +1050,7 @@
         <v>0.91666666666666574</v>
       </c>
       <c r="F29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1230,7 +1071,7 @@
         <v>1.7333333333333323</v>
       </c>
       <c r="F30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1251,7 +1092,7 @@
         <v>1.1833333333333338</v>
       </c>
       <c r="F31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1272,7 +1113,7 @@
         <v>1.3000000000000018</v>
       </c>
       <c r="F32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1293,7 +1134,7 @@
         <v>0.86666666666666592</v>
       </c>
       <c r="F33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1314,7 +1155,7 @@
         <v>0.83333333333333537</v>
       </c>
       <c r="F34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1335,7 +1176,7 @@
         <v>1.0000000000000007</v>
       </c>
       <c r="F35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1356,7 +1197,7 @@
         <v>1.4833333333333354</v>
       </c>
       <c r="F36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1377,7 +1218,7 @@
         <v>0.69999999999999984</v>
       </c>
       <c r="F37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1398,7 +1239,7 @@
         <v>0.54999999999999982</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1419,7 +1260,7 @@
         <v>0.98000000000000043</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1440,7 +1281,7 @@
         <v>0.68333333333333324</v>
       </c>
       <c r="F40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1461,7 +1302,7 @@
         <v>1.1333333333333311</v>
       </c>
       <c r="F41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1482,7 +1323,7 @@
         <v>1.4833333333333361</v>
       </c>
       <c r="F42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1503,7 +1344,7 @@
         <v>2.0833333333333304</v>
       </c>
       <c r="F43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1524,7 +1365,7 @@
         <v>0.91666666666666308</v>
       </c>
       <c r="F44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1545,7 +1386,7 @@
         <v>0.43333333333333329</v>
       </c>
       <c r="F45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1566,7 +1407,7 @@
         <v>1.1666666666666676</v>
       </c>
       <c r="F46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1587,7 +1428,7 @@
         <v>0.48333333333333311</v>
       </c>
       <c r="F47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1608,14 +1449,14 @@
         <v>1.1333333333333309</v>
       </c>
       <c r="F48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>41899</v>
       </c>
-      <c r="B49" s="13">
+      <c r="B49" s="11">
         <v>0.57777777777777783</v>
       </c>
       <c r="C49" s="1">
@@ -1629,7 +1470,7 @@
         <v>0.58333333333333126</v>
       </c>
       <c r="F49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1650,7 +1491,7 @@
         <v>0.26666666666666838</v>
       </c>
       <c r="F50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1671,7 +1512,7 @@
         <v>2.0499999999999994</v>
       </c>
       <c r="F51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1692,7 +1533,7 @@
         <v>1.6833333333333316</v>
       </c>
       <c r="F52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1713,7 +1554,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="F53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1734,7 +1575,7 @@
         <v>1.0666666666666675</v>
       </c>
       <c r="F54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1755,7 +1596,7 @@
         <v>0.38333333333333408</v>
       </c>
       <c r="F55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1776,7 +1617,7 @@
         <v>1.7833333333333332</v>
       </c>
       <c r="F56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1797,7 +1638,7 @@
         <v>0.33333333333333215</v>
       </c>
       <c r="F57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1818,7 +1659,7 @@
         <v>2.9999999999999987</v>
       </c>
       <c r="F58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1839,7 +1680,7 @@
         <v>1.6833333333333347</v>
       </c>
       <c r="F59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1860,7 +1701,7 @@
         <v>1.8500000000000005</v>
       </c>
       <c r="F60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1881,7 +1722,7 @@
         <v>0.34999999999999609</v>
       </c>
       <c r="F61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1902,7 +1743,7 @@
         <v>1.5666666666666662</v>
       </c>
       <c r="F62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1923,7 +1764,7 @@
         <v>0.94999999999999818</v>
       </c>
       <c r="F63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1944,7 +1785,7 @@
         <v>0.61666666666666925</v>
       </c>
       <c r="F64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,7 +1806,7 @@
         <v>0.93333333333333235</v>
       </c>
       <c r="F65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1986,7 +1827,7 @@
         <v>1.0166666666666675</v>
       </c>
       <c r="F66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2007,7 +1848,7 @@
         <v>1.049999999999998</v>
       </c>
       <c r="F67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2028,7 +1869,7 @@
         <v>0.11666666666666625</v>
       </c>
       <c r="F68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2049,7 +1890,7 @@
         <v>1.7333333333333314</v>
       </c>
       <c r="F69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2070,7 +1911,7 @@
         <v>0.95000000000000107</v>
       </c>
       <c r="F70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2091,7 +1932,7 @@
         <v>4.0000000000000027</v>
       </c>
       <c r="F71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2112,7 +1953,7 @@
         <v>1.1166666666666669</v>
       </c>
       <c r="F72" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2133,7 +1974,7 @@
         <v>0.5166666666666645</v>
       </c>
       <c r="F73" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2154,7 +1995,7 @@
         <v>0.61666666666666625</v>
       </c>
       <c r="F74" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2175,7 +2016,7 @@
         <v>0.483333333333334</v>
       </c>
       <c r="F75" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2196,7 +2037,7 @@
         <v>4.366666666666668</v>
       </c>
       <c r="F76" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2217,7 +2058,7 @@
         <v>0.9499999999999984</v>
       </c>
       <c r="F77" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2238,7 +2079,7 @@
         <v>0.91666666666666763</v>
       </c>
       <c r="F78" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2259,7 +2100,7 @@
         <v>1.9500000000000002</v>
       </c>
       <c r="F79" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2280,7 +2121,7 @@
         <v>1.533333333333335</v>
       </c>
       <c r="F80" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2301,7 +2142,7 @@
         <v>2.216666666666665</v>
       </c>
       <c r="F81" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2322,7 +2163,7 @@
         <v>1.8833333333333337</v>
       </c>
       <c r="F82" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2343,7 +2184,7 @@
         <v>0.86666666666667047</v>
       </c>
       <c r="F83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2364,7 +2205,7 @@
         <v>1.5500000000000007</v>
       </c>
       <c r="F84" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2385,7 +2226,7 @@
         <v>0.3666666666666667</v>
       </c>
       <c r="F85" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2406,7 +2247,7 @@
         <v>0.48333333333333239</v>
       </c>
       <c r="F86" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2427,7 +2268,7 @@
         <v>2.3833333333333315</v>
       </c>
       <c r="F87" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2448,7 +2289,7 @@
         <v>2.6999999999999993</v>
       </c>
       <c r="F88" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2469,7 +2310,7 @@
         <v>2.2499999999999987</v>
       </c>
       <c r="F89" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2490,7 +2331,7 @@
         <v>0.70000000000000284</v>
       </c>
       <c r="F90" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2511,7 +2352,7 @@
         <v>0.36666666666666803</v>
       </c>
       <c r="F91" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2532,7 +2373,7 @@
         <v>2.2666666666666653</v>
       </c>
       <c r="F92" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2553,7 +2394,7 @@
         <v>1.8666666666666669</v>
       </c>
       <c r="F93" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2574,7 +2415,7 @@
         <v>0.9000000000000018</v>
       </c>
       <c r="F94" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2595,7 +2436,7 @@
         <v>1.5666666666666689</v>
       </c>
       <c r="F95" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2616,7 +2457,7 @@
         <v>1.2333333333333341</v>
       </c>
       <c r="F96" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -2637,7 +2478,7 @@
         <v>0.89999999999999647</v>
       </c>
       <c r="F97" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2658,7 +2499,7 @@
         <v>1.333333333333331</v>
       </c>
       <c r="F98" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2679,7 +2520,7 @@
         <v>1</v>
       </c>
       <c r="F99" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2700,7 +2541,7 @@
         <v>0.41666666666666519</v>
       </c>
       <c r="F100" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2721,7 +2562,7 @@
         <v>1.6833333333333353</v>
       </c>
       <c r="F101" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2742,7 +2583,7 @@
         <v>1.1500000000000012</v>
       </c>
       <c r="F102" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2763,7 +2604,7 @@
         <v>1.6166666666666663</v>
       </c>
       <c r="F103" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2784,7 +2625,7 @@
         <v>2.7666666666666675</v>
       </c>
       <c r="F104" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -2805,7 +2646,7 @@
         <v>1.8666666666666669</v>
       </c>
       <c r="F105" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -2826,7 +2667,7 @@
         <v>1.9333333333333316</v>
       </c>
       <c r="F106" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -2847,7 +2688,7 @@
         <v>2.9833333333333343</v>
       </c>
       <c r="F107" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -2868,7 +2709,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="F108" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -2889,7 +2730,7 @@
         <v>1.500000000000002</v>
       </c>
       <c r="F109" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -2910,7 +2751,7 @@
         <v>2.6833333333333331</v>
       </c>
       <c r="F110" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -2931,7 +2772,7 @@
         <v>2.3999999999999986</v>
       </c>
       <c r="F111" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -2952,7 +2793,7 @@
         <v>1.8666666666666671</v>
       </c>
       <c r="F112" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -2973,7 +2814,7 @@
         <v>0.43333333333333418</v>
       </c>
       <c r="F113" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -2994,7 +2835,7 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="F114" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3015,7 +2856,7 @@
         <v>2.4666666666666659</v>
       </c>
       <c r="F115" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3036,7 +2877,7 @@
         <v>2.899999999999999</v>
       </c>
       <c r="F116" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3057,7 +2898,7 @@
         <v>1.1333333333333317</v>
       </c>
       <c r="F117" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3078,7 +2919,7 @@
         <v>0.26666666666666544</v>
       </c>
       <c r="F118" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3099,7 +2940,7 @@
         <v>0.31666666666666793</v>
       </c>
       <c r="F119" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3120,7 +2961,7 @@
         <v>0.6499999999999998</v>
       </c>
       <c r="F120" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3141,7 +2982,7 @@
         <v>2.166666666666667</v>
       </c>
       <c r="F121" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3162,7 +3003,7 @@
         <v>1.0833333333333319</v>
       </c>
       <c r="F122" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3183,11 +3024,29 @@
         <v>2.9166666666666692</v>
       </c>
       <c r="F123" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="2"/>
+      <c r="A124" s="2">
+        <v>41990</v>
+      </c>
+      <c r="B124" s="1">
+        <v>0.85138888888888886</v>
+      </c>
+      <c r="C124" s="1">
+        <v>0.8930555555555556</v>
+      </c>
+      <c r="D124" s="3">
+        <v>5</v>
+      </c>
+      <c r="E124" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91666666666666841</v>
+      </c>
+      <c r="F124" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
@@ -3275,15 +3134,15 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E152" s="4">
         <f>SUM(E2:E151)</f>
-        <v>153.32999999999996</v>
+        <v>154.24666666666661</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E153" s="14"/>
+      <c r="E153" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3293,94 +3152,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" activeCellId="1" sqref="A7 C9"/>
+      <selection sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$151,A2,Sheet1!$E$2:$E$151)</f>
-        <v>1.6166666666666663</v>
-      </c>
-      <c r="C2" s="12">
-        <f>B2/SUM($B$2:$B$5)</f>
-        <v>1.0543707471901561E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$151,A3,Sheet1!$E$2:$E$151)</f>
-        <v>124.66666666666664</v>
-      </c>
-      <c r="C3" s="12">
-        <f>B3/SUM($B$2:$B$5)</f>
-        <v>0.81306115350333696</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$151,A4,Sheet1!$E$2:$E$151)</f>
-        <v>19.799999999999997</v>
-      </c>
-      <c r="C4" s="12">
-        <f>B4/SUM($B$2:$B$5)</f>
-        <v>0.12913324202700058</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="10">
-        <f>SUMIF(Sheet1!$F$2:$F$151,A5,Sheet1!$E$2:$E$151)</f>
-        <v>7.2466666666666653</v>
-      </c>
-      <c r="C5" s="12">
-        <f>B5/SUM($B$2:$B$5)</f>
-        <v>4.7261896997760816E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="10">
-        <f>SUM(B2:B5)</f>
-        <v>153.32999999999998</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added Custom games that can be saved.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Task</t>
+  </si>
+  <si>
+    <t>Preset Games</t>
+  </si>
+  <si>
+    <t>Custom Games</t>
   </si>
 </sst>
 </file>
@@ -428,7 +434,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="F132" sqref="F132"/>
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3049,10 +3055,46 @@
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="2"/>
+      <c r="A125" s="2">
+        <v>41994</v>
+      </c>
+      <c r="B125" s="1">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="C125" s="1">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="D125" s="3">
+        <v>5</v>
+      </c>
+      <c r="E125" s="4">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="F125" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="2"/>
+      <c r="A126" s="2">
+        <v>41996</v>
+      </c>
+      <c r="B126" s="1">
+        <v>0.56527777777777777</v>
+      </c>
+      <c r="C126" s="1">
+        <v>0.61736111111111114</v>
+      </c>
+      <c r="D126" s="3">
+        <v>10</v>
+      </c>
+      <c r="E126" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0833333333333341</v>
+      </c>
+      <c r="F126" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
@@ -3138,7 +3180,7 @@
       </c>
       <c r="E152" s="4">
         <f>SUM(E2:E151)</f>
-        <v>154.24666666666661</v>
+        <v>155.62999999999997</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Renamed single card piles to not have number appended.
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Custom Games</t>
+  </si>
+  <si>
+    <t>Renamed Single Piles</t>
   </si>
 </sst>
 </file>
@@ -434,7 +437,7 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127"/>
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +447,7 @@
     <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="10" bestFit="1" customWidth="1"/>
@@ -3097,7 +3100,25 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="2"/>
+      <c r="A127" s="2">
+        <v>41996</v>
+      </c>
+      <c r="B127" s="1">
+        <v>0.61736111111111114</v>
+      </c>
+      <c r="C127" s="1">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="D127" s="3">
+        <v>0</v>
+      </c>
+      <c r="E127" s="4">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999645E-2</v>
+      </c>
+      <c r="F127" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
@@ -3180,7 +3201,7 @@
       </c>
       <c r="E152" s="4">
         <f>SUM(E2:E151)</f>
-        <v>155.62999999999997</v>
+        <v>155.72999999999996</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>